<commit_message>
Preparation of new scenario parameterisation
Initial changes have been made to cater the model for SDG gap scenarios. A problem remains with defining values for IADJ in 2simulation.inc.
</commit_message>
<xml_diff>
--- a/CGE/NDC calcs.xlsx
+++ b/CGE/NDC calcs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faaiq\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE\CGE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339F14CB-84B0-48C2-BC31-AE2450C65D17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA1A3E2-59D0-46AC-BC8F-37117E7781ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22080" windowHeight="13176" xr2:uid="{5EBF588C-42A6-482F-8AFD-23CB1D692841}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5EBF588C-42A6-482F-8AFD-23CB1D692841}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -553,9 +553,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -563,6 +560,9 @@
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -8007,7 +8007,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F5E90B9-1BE5-48C5-BCAB-7235F456714A}">
   <dimension ref="A1:AG106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
@@ -8032,18 +8032,18 @@
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>3</v>
       </c>
       <c r="I2" s="1">
@@ -8083,22 +8083,22 @@
       <c r="A3" t="s">
         <v>128</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="7">
         <v>2019</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="7">
         <v>320.03615997750302</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="7">
         <v>215.30510847308801</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="7">
         <v>141.75206151727099</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="7">
         <v>82.506877630111603</v>
       </c>
       <c r="H3">
@@ -8168,22 +8168,22 @@
       <c r="A4" t="s">
         <v>128</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="7">
         <v>2019</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <v>20.129516626775501</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="7">
         <v>10.383539243494999</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="7">
         <v>6.70969801826232</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="7">
         <v>3.5078811783386201</v>
       </c>
       <c r="H4">
@@ -8253,22 +8253,22 @@
       <c r="A5" t="s">
         <v>128</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="7">
         <v>2019</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="7">
         <v>4.5022404707790002</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="7">
         <v>4.0283055977565896</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="7">
         <v>8.4068925503012295</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="7">
         <v>1.8039552354655799</v>
       </c>
       <c r="H5">
@@ -8319,22 +8319,22 @@
       <c r="A6" t="s">
         <v>129</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="7">
         <v>2019</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="7">
         <v>8.8691063806019308</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="7">
         <v>12.0529138866151</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="7">
         <v>20.071131907589098</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="7">
         <v>26.452794604797901</v>
       </c>
       <c r="H6">
@@ -8381,22 +8381,22 @@
       <c r="A7" t="s">
         <v>129</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="7">
         <v>2019</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="7">
         <v>10.697911853129501</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="7">
         <v>17.784494424227699</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="7">
         <v>36.659722979560499</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="7">
         <v>29.283978923412999</v>
       </c>
       <c r="H7">
@@ -8443,22 +8443,22 @@
       <c r="A8" t="s">
         <v>129</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="7">
         <v>2019</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="7">
         <v>23.4142369281724</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="7">
         <v>29.7758376156956</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="7">
         <v>51.256586121597302</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="7">
         <v>55.804844640273402</v>
       </c>
       <c r="H8">
@@ -8517,22 +8517,22 @@
       <c r="A9" t="s">
         <v>129</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="7">
         <v>2019</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="7">
         <v>4.3937270537413404</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="7">
         <v>8.8615802291832892</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="7">
         <v>14.4040394779541</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="7">
         <v>28.0873177153134</v>
       </c>
       <c r="H9">
@@ -8598,22 +8598,22 @@
       <c r="A10" t="s">
         <v>129</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="7">
         <v>2019</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="7">
         <v>9.6897365711723193E-2</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="7">
         <v>0.31678514662346702</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="7">
         <v>0.48359373270935802</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="7">
         <v>1.3818351541362</v>
       </c>
       <c r="H10">
@@ -8679,22 +8679,22 @@
       <c r="A11" t="s">
         <v>129</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="7">
         <v>2019</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="7">
         <v>9.6309605474421897E-2</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="7">
         <v>0.31486359063911901</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="7">
         <v>0.48066034886550402</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="7">
         <v>1.37345321565794</v>
       </c>
       <c r="H11">
@@ -8745,22 +8745,22 @@
       <c r="A12" t="s">
         <v>130</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="7">
         <v>2019</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="8">
         <v>2.43642703690703E-7</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="8">
         <v>5.25068851644022E-5</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="8">
         <v>1.5733142235428401E-4</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="8">
         <v>1.21276709724953E-4</v>
       </c>
       <c r="H12">
@@ -8782,22 +8782,22 @@
       <c r="A13" t="s">
         <v>130</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="7">
         <v>2019</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="7">
         <v>33.335975496115097</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="7">
         <v>85.425125519341805</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="7">
         <v>146.520757597087</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="7">
         <v>95.817698444021403</v>
       </c>
       <c r="H13">
@@ -8819,22 +8819,22 @@
       <c r="A14" t="s">
         <v>130</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="7">
         <v>2019</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="7">
         <v>20.318361159544398</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="7">
         <v>21.245444522059</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="7">
         <v>36.004223646856097</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="7">
         <v>46.012380696599898</v>
       </c>
       <c r="H14">
@@ -8856,22 +8856,22 @@
       <c r="A15" t="s">
         <v>130</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="7">
         <v>2019</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="7">
         <v>9.5829159302147904</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="7">
         <v>18.582092237400399</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="7">
         <v>47.911704022644102</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="7">
         <v>33.469641330024899</v>
       </c>
       <c r="H15">
@@ -8893,22 +8893,22 @@
       <c r="A16" t="s">
         <v>130</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="7">
         <v>2019</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="7">
         <v>30.657687842799401</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="7">
         <v>43.2733452897996</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="7">
         <v>59.452810650154497</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="7">
         <v>39.148057667851397</v>
       </c>
       <c r="H16">
@@ -8930,22 +8930,22 @@
       <c r="A17" t="s">
         <v>130</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" s="7">
         <v>2019</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D17" s="7">
         <v>0.145195988961835</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="7">
         <v>3.3281897323009999</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F17" s="7">
         <v>12.6904857286798</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="7">
         <v>2.4734101268472699</v>
       </c>
       <c r="H17">
@@ -8979,22 +8979,22 @@
       <c r="A18" t="s">
         <v>130</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="7">
         <v>2019</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D18" s="7">
         <v>2.6093302616715301</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="7">
         <v>11.0224780973285</v>
       </c>
-      <c r="F18" s="8">
+      <c r="F18" s="7">
         <v>15.7041175820872</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G18" s="7">
         <v>13.4943252879869</v>
       </c>
       <c r="H18">
@@ -9035,22 +9035,22 @@
       <c r="A19" t="s">
         <v>130</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" s="7">
         <v>2019</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="8">
+      <c r="D19" s="7">
         <v>15.008240241162</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="7">
         <v>27.291684197519398</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F19" s="7">
         <v>31.6844960984571</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="7">
         <v>14.271382826079</v>
       </c>
       <c r="H19">
@@ -9091,22 +9091,22 @@
       <c r="A20" t="s">
         <v>130</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20" s="7">
         <v>2019</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D20" s="7">
         <v>2.1938463058222899</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="7">
         <v>10.412131518310099</v>
       </c>
-      <c r="F20" s="8">
+      <c r="F20" s="7">
         <v>22.728257842131001</v>
       </c>
-      <c r="G20" s="8">
+      <c r="G20" s="7">
         <v>35.700353058137502</v>
       </c>
       <c r="H20">
@@ -9132,22 +9132,22 @@
       <c r="A21" t="s">
         <v>130</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21" s="7">
         <v>2019</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="8">
+      <c r="D21" s="7">
         <v>7.0064580790196</v>
       </c>
-      <c r="E21" s="8">
+      <c r="E21" s="7">
         <v>17.170599183079101</v>
       </c>
-      <c r="F21" s="8">
+      <c r="F21" s="7">
         <v>47.078662034235002</v>
       </c>
-      <c r="G21" s="8">
+      <c r="G21" s="7">
         <v>63.412124214646802</v>
       </c>
       <c r="H21">
@@ -9169,22 +9169,22 @@
       <c r="A22" t="s">
         <v>130</v>
       </c>
-      <c r="B22" s="8">
+      <c r="B22" s="7">
         <v>2019</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="8">
+      <c r="D22" s="7">
         <v>0.92210654968529204</v>
       </c>
-      <c r="E22" s="8">
+      <c r="E22" s="7">
         <v>3.96944009146983</v>
       </c>
-      <c r="F22" s="8">
+      <c r="F22" s="7">
         <v>8.6238024750236004</v>
       </c>
-      <c r="G22" s="8">
+      <c r="G22" s="7">
         <v>27.716467369360799</v>
       </c>
       <c r="H22">
@@ -9218,22 +9218,22 @@
       <c r="A23" t="s">
         <v>130</v>
       </c>
-      <c r="B23" s="8">
+      <c r="B23" s="7">
         <v>2019</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="7">
         <v>6.75457727352822E-2</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="7">
         <v>8.8906659279458395</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="7">
         <v>26.199302773338701</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="7">
         <v>16.739026996975198</v>
       </c>
       <c r="H23">
@@ -9274,22 +9274,22 @@
       <c r="A24" t="s">
         <v>130</v>
       </c>
-      <c r="B24" s="8">
+      <c r="B24" s="7">
         <v>2019</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="8">
+      <c r="D24" s="7">
         <v>4.8677238364981097</v>
       </c>
-      <c r="E24" s="8">
+      <c r="E24" s="7">
         <v>12.4008746915252</v>
       </c>
-      <c r="F24" s="8">
+      <c r="F24" s="7">
         <v>31.694423635291798</v>
       </c>
-      <c r="G24" s="8">
+      <c r="G24" s="7">
         <v>53.4377512790591</v>
       </c>
       <c r="H24">
@@ -9330,22 +9330,22 @@
       <c r="A25" t="s">
         <v>130</v>
       </c>
-      <c r="B25" s="8">
+      <c r="B25" s="7">
         <v>2019</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="8">
+      <c r="D25" s="7">
         <v>1.2111947984390099</v>
       </c>
-      <c r="E25" s="8">
+      <c r="E25" s="7">
         <v>3.8428273802216601</v>
       </c>
-      <c r="F25" s="8">
+      <c r="F25" s="7">
         <v>8.6963016365446393</v>
       </c>
-      <c r="G25" s="8">
+      <c r="G25" s="7">
         <v>5.4968936886304904</v>
       </c>
       <c r="H25">
@@ -9371,22 +9371,22 @@
       <c r="A26" t="s">
         <v>130</v>
       </c>
-      <c r="B26" s="8">
+      <c r="B26" s="7">
         <v>2019</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="8">
+      <c r="D26" s="7">
         <v>3.4059363864575398</v>
       </c>
-      <c r="E26" s="8">
+      <c r="E26" s="7">
         <v>17.480470291156202</v>
       </c>
-      <c r="F26" s="8">
+      <c r="F26" s="7">
         <v>32.884951393086098</v>
       </c>
-      <c r="G26" s="8">
+      <c r="G26" s="7">
         <v>23.621485241629198</v>
       </c>
       <c r="H26">
@@ -9408,22 +9408,22 @@
       <c r="A27" t="s">
         <v>130</v>
       </c>
-      <c r="B27" s="8">
+      <c r="B27" s="7">
         <v>2019</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="8">
+      <c r="D27" s="7">
         <v>0.926251322297307</v>
       </c>
-      <c r="E27" s="8">
+      <c r="E27" s="7">
         <v>9.2069186848470199</v>
       </c>
-      <c r="F27" s="8">
+      <c r="F27" s="7">
         <v>24.160819943017401</v>
       </c>
-      <c r="G27" s="8">
+      <c r="G27" s="7">
         <v>9.5484015089754006</v>
       </c>
       <c r="H27">
@@ -9445,22 +9445,22 @@
       <c r="A28" t="s">
         <v>130</v>
       </c>
-      <c r="B28" s="8">
+      <c r="B28" s="7">
         <v>2019</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="8">
+      <c r="D28" s="7">
         <v>21.529186395088299</v>
       </c>
-      <c r="E28" s="8">
+      <c r="E28" s="7">
         <v>28.858899281323001</v>
       </c>
-      <c r="F28" s="8">
+      <c r="F28" s="7">
         <v>20.813434509555801</v>
       </c>
-      <c r="G28" s="8">
+      <c r="G28" s="7">
         <v>24.3453287421233</v>
       </c>
       <c r="H28">
@@ -9482,22 +9482,22 @@
       <c r="A29" t="s">
         <v>130</v>
       </c>
-      <c r="B29" s="8">
+      <c r="B29" s="7">
         <v>2019</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D29" s="8">
+      <c r="D29" s="7">
         <v>17.7635532213523</v>
       </c>
-      <c r="E29" s="8">
+      <c r="E29" s="7">
         <v>46.096986409575798</v>
       </c>
-      <c r="F29" s="8">
+      <c r="F29" s="7">
         <v>52.698172132341497</v>
       </c>
-      <c r="G29" s="8">
+      <c r="G29" s="7">
         <v>18.573368795377402</v>
       </c>
       <c r="H29">
@@ -9519,22 +9519,22 @@
       <c r="A30" t="s">
         <v>130</v>
       </c>
-      <c r="B30" s="8">
+      <c r="B30" s="7">
         <v>2019</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="7">
         <v>0.64134182192051603</v>
       </c>
-      <c r="E30" s="8">
+      <c r="E30" s="7">
         <v>1.3414344318871101</v>
       </c>
-      <c r="F30" s="8">
+      <c r="F30" s="7">
         <v>4.1584589166975698</v>
       </c>
-      <c r="G30" s="8">
+      <c r="G30" s="7">
         <v>5.3244589694191697</v>
       </c>
       <c r="H30">
@@ -9556,22 +9556,22 @@
       <c r="A31" t="s">
         <v>130</v>
       </c>
-      <c r="B31" s="8">
+      <c r="B31" s="7">
         <v>2019</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C31" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D31" s="8">
+      <c r="D31" s="7">
         <v>27.019473254573398</v>
       </c>
-      <c r="E31" s="8">
+      <c r="E31" s="7">
         <v>61.1561886780325</v>
       </c>
-      <c r="F31" s="8">
+      <c r="F31" s="7">
         <v>95.237373343533307</v>
       </c>
-      <c r="G31" s="8">
+      <c r="G31" s="7">
         <v>66.454756861625995</v>
       </c>
       <c r="H31">
@@ -9593,22 +9593,22 @@
       <c r="A32" t="s">
         <v>130</v>
       </c>
-      <c r="B32" s="8">
+      <c r="B32" s="7">
         <v>2019</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D32" s="8">
+      <c r="D32" s="7">
         <v>9.8980696996630204</v>
       </c>
-      <c r="E32" s="8">
+      <c r="E32" s="7">
         <v>21.7769182481026</v>
       </c>
-      <c r="F32" s="8">
+      <c r="F32" s="7">
         <v>51.522417803705302</v>
       </c>
-      <c r="G32" s="8">
+      <c r="G32" s="7">
         <v>75.576268103697601</v>
       </c>
       <c r="H32">
@@ -9630,22 +9630,22 @@
       <c r="A33" t="s">
         <v>130</v>
       </c>
-      <c r="B33" s="8">
+      <c r="B33" s="7">
         <v>2019</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D33" s="8">
+      <c r="D33" s="7">
         <v>6.5051765400803898</v>
       </c>
-      <c r="E33" s="8">
+      <c r="E33" s="7">
         <v>14.024065115734199</v>
       </c>
-      <c r="F33" s="8">
+      <c r="F33" s="7">
         <v>13.4829350642232</v>
       </c>
-      <c r="G33" s="8">
+      <c r="G33" s="7">
         <v>14.048015497483499</v>
       </c>
       <c r="H33">
@@ -9667,22 +9667,22 @@
       <c r="A34" t="s">
         <v>130</v>
       </c>
-      <c r="B34" s="8">
+      <c r="B34" s="7">
         <v>2019</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D34" s="8">
+      <c r="D34" s="7">
         <v>0.127767566969549</v>
       </c>
-      <c r="E34" s="8">
+      <c r="E34" s="7">
         <v>2.7198881774545298</v>
       </c>
-      <c r="F34" s="8">
+      <c r="F34" s="7">
         <v>0.83611835211091301</v>
       </c>
-      <c r="G34" s="8">
+      <c r="G34" s="7">
         <v>4.0573964874625901</v>
       </c>
       <c r="H34">
@@ -9704,22 +9704,22 @@
       <c r="A35" t="s">
         <v>130</v>
       </c>
-      <c r="B35" s="8">
+      <c r="B35" s="7">
         <v>2019</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D35" s="8">
+      <c r="D35" s="7">
         <v>13.2133835119593</v>
       </c>
-      <c r="E35" s="8">
+      <c r="E35" s="7">
         <v>11.050163377092</v>
       </c>
-      <c r="F35" s="8">
+      <c r="F35" s="7">
         <v>17.940258029629501</v>
       </c>
-      <c r="G35" s="8">
+      <c r="G35" s="7">
         <v>44.537825618851798</v>
       </c>
       <c r="H35">
@@ -9741,20 +9741,20 @@
       <c r="A36" t="s">
         <v>130</v>
       </c>
-      <c r="B36" s="8">
+      <c r="B36" s="7">
         <v>2019</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8">
+      <c r="D36" s="7"/>
+      <c r="E36" s="7">
         <v>45.888056293725803</v>
       </c>
-      <c r="F36" s="8">
+      <c r="F36" s="7">
         <v>37.2110410657763</v>
       </c>
-      <c r="G36" s="8">
+      <c r="G36" s="7">
         <v>74.4050490131863</v>
       </c>
       <c r="H36">
@@ -9776,22 +9776,22 @@
       <c r="A37" t="s">
         <v>130</v>
       </c>
-      <c r="B37" s="8">
+      <c r="B37" s="7">
         <v>2019</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D37" s="8">
+      <c r="D37" s="7">
         <v>12.284926132604999</v>
       </c>
-      <c r="E37" s="8">
+      <c r="E37" s="7">
         <v>12.8573225808407</v>
       </c>
-      <c r="F37" s="8">
+      <c r="F37" s="7">
         <v>23.836437465797701</v>
       </c>
-      <c r="G37" s="8">
+      <c r="G37" s="7">
         <v>7.1081567318387497</v>
       </c>
       <c r="H37">
@@ -9813,22 +9813,22 @@
       <c r="A38" t="s">
         <v>130</v>
       </c>
-      <c r="B38" s="8">
+      <c r="B38" s="7">
         <v>2019</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C38" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D38" s="8">
+      <c r="D38" s="7">
         <v>4.2310169715642099</v>
       </c>
-      <c r="E38" s="8">
+      <c r="E38" s="7">
         <v>6.4688736462546297</v>
       </c>
-      <c r="F38" s="8">
+      <c r="F38" s="7">
         <v>17.852806962322099</v>
       </c>
-      <c r="G38" s="8">
+      <c r="G38" s="7">
         <v>16.802593249859701</v>
       </c>
       <c r="H38">
@@ -9850,22 +9850,22 @@
       <c r="A39" t="s">
         <v>131</v>
       </c>
-      <c r="B39" s="8">
+      <c r="B39" s="7">
         <v>2019</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D39" s="8">
+      <c r="D39" s="7">
         <v>3.6451330920735501</v>
       </c>
-      <c r="E39" s="8">
+      <c r="E39" s="7">
         <v>4.14843396492582</v>
       </c>
-      <c r="F39" s="8">
+      <c r="F39" s="7">
         <v>13.7256572868442</v>
       </c>
-      <c r="G39" s="8">
+      <c r="G39" s="7">
         <v>49.1390816422835</v>
       </c>
       <c r="H39">
@@ -9887,22 +9887,22 @@
       <c r="A40" t="s">
         <v>131</v>
       </c>
-      <c r="B40" s="8">
+      <c r="B40" s="7">
         <v>2019</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C40" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D40" s="8">
+      <c r="D40" s="7">
         <v>6.8280647070468001</v>
       </c>
-      <c r="E40" s="8">
+      <c r="E40" s="7">
         <v>7.6462452280383202</v>
       </c>
-      <c r="F40" s="8">
+      <c r="F40" s="7">
         <v>9.6536127147516009</v>
       </c>
-      <c r="G40" s="8">
+      <c r="G40" s="7">
         <v>10.5614314974596</v>
       </c>
       <c r="H40">
@@ -9924,22 +9924,22 @@
       <c r="A41" t="s">
         <v>132</v>
       </c>
-      <c r="B41" s="8">
+      <c r="B41" s="7">
         <v>2019</v>
       </c>
-      <c r="C41" s="8" t="s">
+      <c r="C41" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D41" s="8">
+      <c r="D41" s="7">
         <v>293.67147194941703</v>
       </c>
-      <c r="E41" s="8">
+      <c r="E41" s="7">
         <v>370.53306262399002</v>
       </c>
-      <c r="F41" s="8">
+      <c r="F41" s="7">
         <v>448.35990570931102</v>
       </c>
-      <c r="G41" s="8">
+      <c r="G41" s="7">
         <v>320.27915632044102</v>
       </c>
       <c r="H41">
@@ -9961,22 +9961,22 @@
       <c r="A42" t="s">
         <v>133</v>
       </c>
-      <c r="B42" s="8">
+      <c r="B42" s="7">
         <v>2019</v>
       </c>
-      <c r="C42" s="8" t="s">
+      <c r="C42" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D42" s="8">
+      <c r="D42" s="7">
         <v>319.58357088925101</v>
       </c>
-      <c r="E42" s="8">
+      <c r="E42" s="7">
         <v>555.00069577868999</v>
       </c>
-      <c r="F42" s="8">
+      <c r="F42" s="7">
         <v>1028.6425186434799</v>
       </c>
-      <c r="G42" s="8">
+      <c r="G42" s="7">
         <v>841.81079611443295</v>
       </c>
       <c r="H42">
@@ -9998,22 +9998,22 @@
       <c r="A43" t="s">
         <v>133</v>
       </c>
-      <c r="B43" s="8">
+      <c r="B43" s="7">
         <v>2019</v>
       </c>
-      <c r="C43" s="8" t="s">
+      <c r="C43" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D43" s="8">
+      <c r="D43" s="7">
         <v>44.150793339386901</v>
       </c>
-      <c r="E43" s="8">
+      <c r="E43" s="7">
         <v>108.197876704002</v>
       </c>
-      <c r="F43" s="8">
+      <c r="F43" s="7">
         <v>268.25021856928498</v>
       </c>
-      <c r="G43" s="8">
+      <c r="G43" s="7">
         <v>202.020888055683</v>
       </c>
       <c r="H43">
@@ -10035,22 +10035,22 @@
       <c r="A44" t="s">
         <v>134</v>
       </c>
-      <c r="B44" s="8">
+      <c r="B44" s="7">
         <v>2019</v>
       </c>
-      <c r="C44" s="8" t="s">
+      <c r="C44" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D44" s="8">
+      <c r="D44" s="7">
         <v>3.7382387815879898</v>
       </c>
-      <c r="E44" s="8">
+      <c r="E44" s="7">
         <v>6.9322710593493504</v>
       </c>
-      <c r="F44" s="8">
+      <c r="F44" s="7">
         <v>22.5996300520329</v>
       </c>
-      <c r="G44" s="8">
+      <c r="G44" s="7">
         <v>27.172710951292999</v>
       </c>
       <c r="H44">
@@ -10072,22 +10072,22 @@
       <c r="A45" t="s">
         <v>134</v>
       </c>
-      <c r="B45" s="8">
+      <c r="B45" s="7">
         <v>2019</v>
       </c>
-      <c r="C45" s="8" t="s">
+      <c r="C45" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D45" s="8">
+      <c r="D45" s="7">
         <v>8.6908938728554403</v>
       </c>
-      <c r="E45" s="8">
+      <c r="E45" s="7">
         <v>17.173996145700499</v>
       </c>
-      <c r="F45" s="8">
+      <c r="F45" s="7">
         <v>18.828025089179</v>
       </c>
-      <c r="G45" s="8">
+      <c r="G45" s="7">
         <v>10.2582520575874</v>
       </c>
       <c r="H45">
@@ -10109,22 +10109,22 @@
       <c r="A46" t="s">
         <v>134</v>
       </c>
-      <c r="B46" s="8">
+      <c r="B46" s="7">
         <v>2019</v>
       </c>
-      <c r="C46" s="8" t="s">
+      <c r="C46" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D46" s="8">
+      <c r="D46" s="7">
         <v>38.392223061426897</v>
       </c>
-      <c r="E46" s="8">
+      <c r="E46" s="7">
         <v>75.866521962799396</v>
       </c>
-      <c r="F46" s="8">
+      <c r="F46" s="7">
         <v>83.173232765742597</v>
       </c>
-      <c r="G46" s="8">
+      <c r="G46" s="7">
         <v>45.316063799339098</v>
       </c>
       <c r="H46">
@@ -10146,20 +10146,20 @@
       <c r="A47" t="s">
         <v>134</v>
       </c>
-      <c r="B47" s="8">
+      <c r="B47" s="7">
         <v>2019</v>
       </c>
-      <c r="C47" s="8" t="s">
+      <c r="C47" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D47" s="8"/>
-      <c r="E47" s="8">
+      <c r="D47" s="7"/>
+      <c r="E47" s="7">
         <v>1.15497477153172E-3</v>
       </c>
-      <c r="F47" s="8">
+      <c r="F47" s="7">
         <v>0.17409872813751001</v>
       </c>
-      <c r="G47" s="8">
+      <c r="G47" s="7">
         <v>0.14656971112988601</v>
       </c>
       <c r="H47">
@@ -10181,22 +10181,22 @@
       <c r="A48" t="s">
         <v>134</v>
       </c>
-      <c r="B48" s="8">
+      <c r="B48" s="7">
         <v>2019</v>
       </c>
-      <c r="C48" s="8" t="s">
+      <c r="C48" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D48" s="8">
+      <c r="D48" s="7">
         <v>0.64412515224919398</v>
       </c>
-      <c r="E48" s="8">
+      <c r="E48" s="7">
         <v>0.45996042774142898</v>
       </c>
-      <c r="F48" s="8">
+      <c r="F48" s="7">
         <v>3.2915774135969502</v>
       </c>
-      <c r="G48" s="8">
+      <c r="G48" s="7">
         <v>5.5015659157933303</v>
       </c>
       <c r="H48">
@@ -10218,22 +10218,22 @@
       <c r="A49" t="s">
         <v>134</v>
       </c>
-      <c r="B49" s="8">
+      <c r="B49" s="7">
         <v>2019</v>
       </c>
-      <c r="C49" s="8" t="s">
+      <c r="C49" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D49" s="8">
+      <c r="D49" s="7">
         <v>3.8153630872142799</v>
       </c>
-      <c r="E49" s="8">
+      <c r="E49" s="7">
         <v>15.9722413429709</v>
       </c>
-      <c r="F49" s="8">
+      <c r="F49" s="7">
         <v>60.615739046861201</v>
       </c>
-      <c r="G49" s="8">
+      <c r="G49" s="7">
         <v>108.093304574998</v>
       </c>
       <c r="H49">
@@ -10255,22 +10255,22 @@
       <c r="A50" t="s">
         <v>135</v>
       </c>
-      <c r="B50" s="8">
+      <c r="B50" s="7">
         <v>2019</v>
       </c>
-      <c r="C50" s="8" t="s">
+      <c r="C50" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D50" s="8">
+      <c r="D50" s="7">
         <v>4.6157597838523499</v>
       </c>
-      <c r="E50" s="8">
+      <c r="E50" s="7">
         <v>5.1421380594604402</v>
       </c>
-      <c r="F50" s="8">
+      <c r="F50" s="7">
         <v>104.395127633402</v>
       </c>
-      <c r="G50" s="8">
+      <c r="G50" s="7">
         <v>264.02405477226603</v>
       </c>
       <c r="H50">
@@ -10292,22 +10292,22 @@
       <c r="A51" t="s">
         <v>135</v>
       </c>
-      <c r="B51" s="8">
+      <c r="B51" s="7">
         <v>2019</v>
       </c>
-      <c r="C51" s="8" t="s">
+      <c r="C51" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D51" s="8">
+      <c r="D51" s="7">
         <v>73.234408634515503</v>
       </c>
-      <c r="E51" s="8">
+      <c r="E51" s="7">
         <v>200.176534354122</v>
       </c>
-      <c r="F51" s="8">
+      <c r="F51" s="7">
         <v>544.84865904928097</v>
       </c>
-      <c r="G51" s="8">
+      <c r="G51" s="7">
         <v>660.94237566374795</v>
       </c>
       <c r="H51">
@@ -10329,22 +10329,22 @@
       <c r="A52" t="s">
         <v>136</v>
       </c>
-      <c r="B52" s="8">
+      <c r="B52" s="7">
         <v>2019</v>
       </c>
-      <c r="C52" s="8" t="s">
+      <c r="C52" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D52" s="8">
+      <c r="D52" s="7">
         <v>44.910059839713199</v>
       </c>
-      <c r="E52" s="8">
+      <c r="E52" s="7">
         <v>87.536001613985206</v>
       </c>
-      <c r="F52" s="8">
+      <c r="F52" s="7">
         <v>270.77964438975101</v>
       </c>
-      <c r="G52" s="8">
+      <c r="G52" s="7">
         <v>607.41660599975899</v>
       </c>
       <c r="H52">
@@ -10366,22 +10366,22 @@
       <c r="A53" t="s">
         <v>137</v>
       </c>
-      <c r="B53" s="8">
+      <c r="B53" s="7">
         <v>2019</v>
       </c>
-      <c r="C53" s="8" t="s">
+      <c r="C53" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D53" s="8">
+      <c r="D53" s="7">
         <v>905.78274514289103</v>
       </c>
-      <c r="E53" s="8">
+      <c r="E53" s="7">
         <v>1118.7819759756601</v>
       </c>
-      <c r="F53" s="8">
+      <c r="F53" s="7">
         <v>809.33014088140601</v>
       </c>
-      <c r="G53" s="8">
+      <c r="G53" s="7">
         <v>1417.86125122198</v>
       </c>
       <c r="H53">
@@ -10400,22 +10400,22 @@
       </c>
     </row>
     <row r="54" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="B54" s="8">
+      <c r="B54" s="7">
         <v>2019</v>
       </c>
-      <c r="C54" s="8" t="s">
+      <c r="C54" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D54" s="9">
+      <c r="D54" s="8">
         <v>4.46072734173926E-9</v>
       </c>
-      <c r="E54" s="9">
+      <c r="E54" s="8">
         <v>2.35752304743582E-9</v>
       </c>
-      <c r="F54" s="9">
+      <c r="F54" s="8">
         <v>1.57291547571013E-9</v>
       </c>
-      <c r="G54" s="9">
+      <c r="G54" s="8">
         <v>8.7606719461990603E-10</v>
       </c>
       <c r="H54">
@@ -10434,22 +10434,22 @@
       </c>
     </row>
     <row r="55" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="B55" s="8">
+      <c r="B55" s="7">
         <v>2020</v>
       </c>
-      <c r="C55" s="8" t="s">
+      <c r="C55" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D55" s="8">
+      <c r="D55" s="7">
         <v>269.99606462186398</v>
       </c>
-      <c r="E55" s="8">
+      <c r="E55" s="7">
         <v>181.29739822916801</v>
       </c>
-      <c r="F55" s="8">
+      <c r="F55" s="7">
         <v>119.31682235443</v>
       </c>
-      <c r="G55" s="8">
+      <c r="G55" s="7">
         <v>69.194986671235995</v>
       </c>
       <c r="H55">
@@ -10465,22 +10465,22 @@
       </c>
     </row>
     <row r="56" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="B56" s="8">
+      <c r="B56" s="7">
         <v>2020</v>
       </c>
-      <c r="C56" s="8" t="s">
+      <c r="C56" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D56" s="8">
+      <c r="D56" s="7">
         <v>16.1965313042869</v>
       </c>
-      <c r="E56" s="8">
+      <c r="E56" s="7">
         <v>8.3389799800074709</v>
       </c>
-      <c r="F56" s="8">
+      <c r="F56" s="7">
         <v>5.3864862401553699</v>
       </c>
-      <c r="G56" s="8">
+      <c r="G56" s="7">
         <v>2.80581890670926</v>
       </c>
       <c r="H56">
@@ -10496,22 +10496,22 @@
       </c>
     </row>
     <row r="57" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="B57" s="8">
+      <c r="B57" s="7">
         <v>2020</v>
       </c>
-      <c r="C57" s="8" t="s">
+      <c r="C57" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D57" s="8">
+      <c r="D57" s="7">
         <v>3.8468333582523702</v>
       </c>
-      <c r="E57" s="8">
+      <c r="E57" s="7">
         <v>3.4353892299694202</v>
       </c>
-      <c r="F57" s="8">
+      <c r="F57" s="7">
         <v>7.1667803520975699</v>
       </c>
-      <c r="G57" s="8">
+      <c r="G57" s="7">
         <v>1.5322390874179601</v>
       </c>
       <c r="H57">
@@ -10527,22 +10527,22 @@
       </c>
     </row>
     <row r="58" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="B58" s="8">
+      <c r="B58" s="7">
         <v>2020</v>
       </c>
-      <c r="C58" s="8" t="s">
+      <c r="C58" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D58" s="8">
+      <c r="D58" s="7">
         <v>8.7740441962185294</v>
       </c>
-      <c r="E58" s="8">
+      <c r="E58" s="7">
         <v>11.923726539764299</v>
       </c>
-      <c r="F58" s="8">
+      <c r="F58" s="7">
         <v>19.856002495413399</v>
       </c>
-      <c r="G58" s="8">
+      <c r="G58" s="7">
         <v>26.169264299684301</v>
       </c>
       <c r="H58">
@@ -10558,22 +10558,22 @@
       </c>
     </row>
     <row r="59" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="B59" s="8">
+      <c r="B59" s="7">
         <v>2020</v>
       </c>
-      <c r="C59" s="8" t="s">
+      <c r="C59" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D59" s="8">
+      <c r="D59" s="7">
         <v>10.687213941276299</v>
       </c>
-      <c r="E59" s="8">
+      <c r="E59" s="7">
         <v>17.766709929803401</v>
       </c>
-      <c r="F59" s="8">
+      <c r="F59" s="7">
         <v>36.623063256580899</v>
       </c>
-      <c r="G59" s="8">
+      <c r="G59" s="7">
         <v>29.254694944489501</v>
       </c>
       <c r="H59">
@@ -10589,22 +10589,22 @@
       </c>
     </row>
     <row r="60" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="B60" s="8">
+      <c r="B60" s="7">
         <v>2020</v>
       </c>
-      <c r="C60" s="8" t="s">
+      <c r="C60" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D60" s="8">
+      <c r="D60" s="7">
         <v>19.8212106962301</v>
       </c>
-      <c r="E60" s="8">
+      <c r="E60" s="7">
         <v>25.161213409431902</v>
       </c>
-      <c r="F60" s="8">
+      <c r="F60" s="7">
         <v>43.297226396714997</v>
       </c>
-      <c r="G60" s="8">
+      <c r="G60" s="7">
         <v>46.975246509008301</v>
       </c>
       <c r="H60">
@@ -10620,22 +10620,22 @@
       </c>
     </row>
     <row r="61" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="B61" s="8">
+      <c r="B61" s="7">
         <v>2020</v>
       </c>
-      <c r="C61" s="8" t="s">
+      <c r="C61" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D61" s="8">
+      <c r="D61" s="7">
         <v>3.9024213081650099</v>
       </c>
-      <c r="E61" s="8">
+      <c r="E61" s="7">
         <v>7.8565101951272496</v>
       </c>
-      <c r="F61" s="8">
+      <c r="F61" s="7">
         <v>12.765728774448499</v>
       </c>
-      <c r="G61" s="8">
+      <c r="G61" s="7">
         <v>24.806091538297299</v>
       </c>
       <c r="H61">
@@ -10651,22 +10651,22 @@
       </c>
     </row>
     <row r="62" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="B62" s="8">
+      <c r="B62" s="7">
         <v>2020</v>
       </c>
-      <c r="C62" s="8" t="s">
+      <c r="C62" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D62" s="8">
+      <c r="D62" s="7">
         <v>0.101334054700675</v>
       </c>
-      <c r="E62" s="8">
+      <c r="E62" s="7">
         <v>0.33069352009213998</v>
       </c>
-      <c r="F62" s="8">
+      <c r="F62" s="7">
         <v>0.50464310520312805</v>
       </c>
-      <c r="G62" s="8">
+      <c r="G62" s="7">
         <v>1.4369666280161399</v>
       </c>
       <c r="H62">
@@ -10682,22 +10682,22 @@
       </c>
     </row>
     <row r="63" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="B63" s="8">
+      <c r="B63" s="7">
         <v>2020</v>
       </c>
-      <c r="C63" s="8" t="s">
+      <c r="C63" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D63" s="8">
+      <c r="D63" s="7">
         <v>0.10029203996663701</v>
       </c>
-      <c r="E63" s="8">
+      <c r="E63" s="7">
         <v>0.32729300955888302</v>
       </c>
-      <c r="F63" s="8">
+      <c r="F63" s="7">
         <v>0.499453876837541</v>
       </c>
-      <c r="G63" s="8">
+      <c r="G63" s="7">
         <v>1.4221903476912501</v>
       </c>
       <c r="H63">
@@ -10713,22 +10713,22 @@
       </c>
     </row>
     <row r="64" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="B64" s="8">
+      <c r="B64" s="7">
         <v>2020</v>
       </c>
-      <c r="C64" s="8" t="s">
+      <c r="C64" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D64" s="9">
+      <c r="D64" s="8">
         <v>1.78023351054887E-7</v>
       </c>
-      <c r="E64" s="9">
+      <c r="E64" s="8">
         <v>3.8295173957113198E-5</v>
       </c>
-      <c r="F64" s="9">
+      <c r="F64" s="8">
         <v>1.1470528143211599E-4</v>
       </c>
-      <c r="G64" s="9">
+      <c r="G64" s="8">
         <v>8.8106226624809305E-5</v>
       </c>
       <c r="H64">
@@ -10744,22 +10744,22 @@
       </c>
     </row>
     <row r="65" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B65" s="8">
+      <c r="B65" s="7">
         <v>2020</v>
       </c>
-      <c r="C65" s="8" t="s">
+      <c r="C65" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D65" s="8">
+      <c r="D65" s="7">
         <v>29.9450662672375</v>
       </c>
-      <c r="E65" s="8">
+      <c r="E65" s="7">
         <v>76.595272449051194</v>
       </c>
-      <c r="F65" s="8">
+      <c r="F65" s="7">
         <v>131.32749188391301</v>
       </c>
-      <c r="G65" s="8">
+      <c r="G65" s="7">
         <v>85.5782654042019</v>
       </c>
       <c r="H65">
@@ -10775,22 +10775,22 @@
       </c>
     </row>
     <row r="66" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B66" s="8">
+      <c r="B66" s="7">
         <v>2020</v>
       </c>
-      <c r="C66" s="8" t="s">
+      <c r="C66" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D66" s="8">
+      <c r="D66" s="7">
         <v>17.653913764874702</v>
       </c>
-      <c r="E66" s="8">
+      <c r="E66" s="7">
         <v>18.425631313383999</v>
       </c>
-      <c r="F66" s="8">
+      <c r="F66" s="7">
         <v>31.214052765670498</v>
       </c>
-      <c r="G66" s="8">
+      <c r="G66" s="7">
         <v>39.749590959357803</v>
       </c>
       <c r="H66">
@@ -10806,22 +10806,22 @@
       </c>
     </row>
     <row r="67" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B67" s="8">
+      <c r="B67" s="7">
         <v>2020</v>
       </c>
-      <c r="C67" s="8" t="s">
+      <c r="C67" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D67" s="8">
+      <c r="D67" s="7">
         <v>8.7786951740624897</v>
       </c>
-      <c r="E67" s="8">
+      <c r="E67" s="7">
         <v>16.991476996002898</v>
       </c>
-      <c r="F67" s="8">
+      <c r="F67" s="7">
         <v>43.7943709304839</v>
       </c>
-      <c r="G67" s="8">
+      <c r="G67" s="7">
         <v>30.485195445070399</v>
       </c>
       <c r="H67">
@@ -10837,22 +10837,22 @@
       </c>
     </row>
     <row r="68" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B68" s="8">
+      <c r="B68" s="7">
         <v>2020</v>
       </c>
-      <c r="C68" s="8" t="s">
+      <c r="C68" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D68" s="8">
+      <c r="D68" s="7">
         <v>28.733135824934301</v>
       </c>
-      <c r="E68" s="8">
+      <c r="E68" s="7">
         <v>40.482593479475199</v>
       </c>
-      <c r="F68" s="8">
+      <c r="F68" s="7">
         <v>55.598157955227698</v>
       </c>
-      <c r="G68" s="8">
+      <c r="G68" s="7">
         <v>36.480390763494803</v>
       </c>
       <c r="H68">
@@ -10868,22 +10868,22 @@
       </c>
     </row>
     <row r="69" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B69" s="8">
+      <c r="B69" s="7">
         <v>2020</v>
       </c>
-      <c r="C69" s="8" t="s">
+      <c r="C69" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D69" s="8">
+      <c r="D69" s="7">
         <v>0.13271742678676901</v>
       </c>
-      <c r="E69" s="8">
+      <c r="E69" s="7">
         <v>3.0365863775495301</v>
       </c>
-      <c r="F69" s="8">
+      <c r="F69" s="7">
         <v>11.5743327276919</v>
       </c>
-      <c r="G69" s="8">
+      <c r="G69" s="7">
         <v>2.2478902442830502</v>
       </c>
       <c r="H69">
@@ -10899,22 +10899,22 @@
       </c>
     </row>
     <row r="70" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B70" s="8">
+      <c r="B70" s="7">
         <v>2020</v>
       </c>
-      <c r="C70" s="8" t="s">
+      <c r="C70" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D70" s="8">
+      <c r="D70" s="7">
         <v>2.50041147410756</v>
       </c>
-      <c r="E70" s="8">
+      <c r="E70" s="7">
         <v>10.5430412585846</v>
       </c>
-      <c r="F70" s="8">
+      <c r="F70" s="7">
         <v>15.015519237880101</v>
       </c>
-      <c r="G70" s="8">
+      <c r="G70" s="7">
         <v>12.8569880828134</v>
       </c>
       <c r="H70">
@@ -10930,22 +10930,22 @@
       </c>
     </row>
     <row r="71" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B71" s="8">
+      <c r="B71" s="7">
         <v>2020</v>
       </c>
-      <c r="C71" s="8" t="s">
+      <c r="C71" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D71" s="8">
+      <c r="D71" s="7">
         <v>13.1663122292374</v>
       </c>
-      <c r="E71" s="8">
+      <c r="E71" s="7">
         <v>23.898406475263101</v>
       </c>
-      <c r="F71" s="8">
+      <c r="F71" s="7">
         <v>27.734833675121401</v>
       </c>
-      <c r="G71" s="8">
+      <c r="G71" s="7">
         <v>12.4481859565006</v>
       </c>
       <c r="H71">
@@ -10961,22 +10961,22 @@
       </c>
     </row>
     <row r="72" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B72" s="8">
+      <c r="B72" s="7">
         <v>2020</v>
       </c>
-      <c r="C72" s="8" t="s">
+      <c r="C72" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D72" s="8">
+      <c r="D72" s="7">
         <v>1.9120664099784801</v>
       </c>
-      <c r="E72" s="8">
+      <c r="E72" s="7">
         <v>9.0581737681032699</v>
       </c>
-      <c r="F72" s="8">
+      <c r="F72" s="7">
         <v>19.765477248082</v>
       </c>
-      <c r="G72" s="8">
+      <c r="G72" s="7">
         <v>30.936766442960199</v>
       </c>
       <c r="H72">
@@ -10992,22 +10992,22 @@
       </c>
     </row>
     <row r="73" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B73" s="8">
+      <c r="B73" s="7">
         <v>2020</v>
       </c>
-      <c r="C73" s="8" t="s">
+      <c r="C73" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D73" s="8">
+      <c r="D73" s="7">
         <v>6.7449740414310799</v>
       </c>
-      <c r="E73" s="8">
+      <c r="E73" s="7">
         <v>16.499524734536902</v>
       </c>
-      <c r="F73" s="8">
+      <c r="F73" s="7">
         <v>45.222050514265703</v>
       </c>
-      <c r="G73" s="8">
+      <c r="G73" s="7">
         <v>60.695946848533303</v>
       </c>
       <c r="H73">
@@ -11023,22 +11023,22 @@
       </c>
     </row>
     <row r="74" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B74" s="8">
+      <c r="B74" s="7">
         <v>2020</v>
       </c>
-      <c r="C74" s="8" t="s">
+      <c r="C74" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D74" s="8">
+      <c r="D74" s="7">
         <v>0.91935811044231697</v>
       </c>
-      <c r="E74" s="8">
+      <c r="E74" s="7">
         <v>3.95760874191076</v>
       </c>
-      <c r="F74" s="8">
+      <c r="F74" s="7">
         <v>8.5980982902370204</v>
       </c>
-      <c r="G74" s="8">
+      <c r="G74" s="7">
         <v>27.633855412401399</v>
       </c>
       <c r="H74">
@@ -11054,22 +11054,22 @@
       </c>
     </row>
     <row r="75" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B75" s="8">
+      <c r="B75" s="7">
         <v>2020</v>
       </c>
-      <c r="C75" s="8" t="s">
+      <c r="C75" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D75" s="8">
+      <c r="D75" s="7">
         <v>5.9865463347908598E-2</v>
       </c>
-      <c r="E75" s="8">
+      <c r="E75" s="7">
         <v>7.8653254022146797</v>
       </c>
-      <c r="F75" s="8">
+      <c r="F75" s="7">
         <v>23.169266868852301</v>
       </c>
-      <c r="G75" s="8">
+      <c r="G75" s="7">
         <v>14.750747126839601</v>
       </c>
       <c r="H75">
@@ -11079,22 +11079,22 @@
       <c r="I75" s="1"/>
     </row>
     <row r="76" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B76" s="8">
+      <c r="B76" s="7">
         <v>2020</v>
       </c>
-      <c r="C76" s="8" t="s">
+      <c r="C76" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D76" s="8">
+      <c r="D76" s="7">
         <v>4.4768537439751404</v>
       </c>
-      <c r="E76" s="8">
+      <c r="E76" s="7">
         <v>11.384226393062001</v>
       </c>
-      <c r="F76" s="8">
+      <c r="F76" s="7">
         <v>29.085344899222999</v>
       </c>
-      <c r="G76" s="8">
+      <c r="G76" s="7">
         <v>48.865324139600098</v>
       </c>
       <c r="H76">
@@ -11104,22 +11104,22 @@
       <c r="I76" s="1"/>
     </row>
     <row r="77" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B77" s="8">
+      <c r="B77" s="7">
         <v>2020</v>
       </c>
-      <c r="C77" s="8" t="s">
+      <c r="C77" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D77" s="8">
+      <c r="D77" s="7">
         <v>1.0697579157028101</v>
       </c>
-      <c r="E77" s="8">
+      <c r="E77" s="7">
         <v>3.3878690666171098</v>
       </c>
-      <c r="F77" s="8">
+      <c r="F77" s="7">
         <v>7.6639116773015301</v>
       </c>
-      <c r="G77" s="8">
+      <c r="G77" s="7">
         <v>4.8271910068474604</v>
       </c>
       <c r="H77">
@@ -11129,22 +11129,22 @@
       <c r="I77" s="1"/>
     </row>
     <row r="78" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B78" s="8">
+      <c r="B78" s="7">
         <v>2020</v>
       </c>
-      <c r="C78" s="8" t="s">
+      <c r="C78" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D78" s="8">
+      <c r="D78" s="7">
         <v>3.1455300567377802</v>
       </c>
-      <c r="E78" s="8">
+      <c r="E78" s="7">
         <v>16.1144189022746</v>
       </c>
-      <c r="F78" s="8">
+      <c r="F78" s="7">
         <v>30.303925920005799</v>
       </c>
-      <c r="G78" s="8">
+      <c r="G78" s="7">
         <v>21.6905289344407</v>
       </c>
       <c r="H78">
@@ -11154,22 +11154,22 @@
       <c r="I78" s="1"/>
     </row>
     <row r="79" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B79" s="8">
+      <c r="B79" s="7">
         <v>2020</v>
       </c>
-      <c r="C79" s="8" t="s">
+      <c r="C79" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D79" s="8">
+      <c r="D79" s="7">
         <v>0.88990038285473305</v>
       </c>
-      <c r="E79" s="8">
+      <c r="E79" s="7">
         <v>8.8293979130663196</v>
       </c>
-      <c r="F79" s="8">
+      <c r="F79" s="7">
         <v>23.161602593091299</v>
       </c>
-      <c r="G79" s="8">
+      <c r="G79" s="7">
         <v>9.1211344973666595</v>
       </c>
       <c r="H79">
@@ -11179,22 +11179,22 @@
       <c r="I79" s="1"/>
     </row>
     <row r="80" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B80" s="8">
+      <c r="B80" s="7">
         <v>2020</v>
       </c>
-      <c r="C80" s="8" t="s">
+      <c r="C80" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D80" s="8">
+      <c r="D80" s="7">
         <v>18.496008851394301</v>
       </c>
-      <c r="E80" s="8">
+      <c r="E80" s="7">
         <v>24.747674695911201</v>
       </c>
-      <c r="F80" s="8">
+      <c r="F80" s="7">
         <v>17.841794868590998</v>
       </c>
-      <c r="G80" s="8">
+      <c r="G80" s="7">
         <v>20.795610975265401</v>
       </c>
       <c r="H80">
@@ -11204,22 +11204,22 @@
       <c r="I80" s="1"/>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B81" s="8">
+      <c r="B81" s="7">
         <v>2020</v>
       </c>
-      <c r="C81" s="8" t="s">
+      <c r="C81" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D81" s="8">
+      <c r="D81" s="7">
         <v>17.203363891859201</v>
       </c>
-      <c r="E81" s="8">
+      <c r="E81" s="7">
         <v>44.561550960174102</v>
       </c>
-      <c r="F81" s="8">
+      <c r="F81" s="7">
         <v>50.924112659951703</v>
       </c>
-      <c r="G81" s="8">
+      <c r="G81" s="7">
         <v>17.8846255132095</v>
       </c>
       <c r="H81">
@@ -11229,22 +11229,22 @@
       <c r="I81" s="1"/>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B82" s="8">
+      <c r="B82" s="7">
         <v>2020</v>
       </c>
-      <c r="C82" s="8" t="s">
+      <c r="C82" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D82" s="8">
+      <c r="D82" s="7">
         <v>0.530159391617536</v>
       </c>
-      <c r="E82" s="8">
+      <c r="E82" s="7">
         <v>1.1068546069384699</v>
       </c>
-      <c r="F82" s="8">
+      <c r="F82" s="7">
         <v>3.42999666307922</v>
       </c>
-      <c r="G82" s="8">
+      <c r="G82" s="7">
         <v>4.3762086181653501</v>
       </c>
       <c r="H82">
@@ -11254,22 +11254,22 @@
       <c r="I82" s="1"/>
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B83" s="8">
+      <c r="B83" s="7">
         <v>2020</v>
       </c>
-      <c r="C83" s="8" t="s">
+      <c r="C83" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D83" s="8">
+      <c r="D83" s="7">
         <v>26.9163201171447</v>
       </c>
-      <c r="E83" s="8">
+      <c r="E83" s="7">
         <v>60.8111824015308</v>
       </c>
-      <c r="F83" s="8">
+      <c r="F83" s="7">
         <v>94.665252985638602</v>
       </c>
-      <c r="G83" s="8">
+      <c r="G83" s="7">
         <v>65.821915145440201</v>
       </c>
       <c r="H83">
@@ -11279,22 +11279,22 @@
       <c r="I83" s="1"/>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B84" s="8">
+      <c r="B84" s="7">
         <v>2020</v>
       </c>
-      <c r="C84" s="8" t="s">
+      <c r="C84" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D84" s="8">
+      <c r="D84" s="7">
         <v>9.6454936890920493</v>
       </c>
-      <c r="E84" s="8">
+      <c r="E84" s="7">
         <v>21.182372631844501</v>
       </c>
-      <c r="F84" s="8">
+      <c r="F84" s="7">
         <v>50.097329153358899</v>
       </c>
-      <c r="G84" s="8">
+      <c r="G84" s="7">
         <v>73.225952725967602</v>
       </c>
       <c r="H84">
@@ -11304,22 +11304,22 @@
       <c r="I84" s="1"/>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B85" s="8">
+      <c r="B85" s="7">
         <v>2020</v>
       </c>
-      <c r="C85" s="8" t="s">
+      <c r="C85" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D85" s="8">
+      <c r="D85" s="7">
         <v>6.4264367471714996</v>
       </c>
-      <c r="E85" s="8">
+      <c r="E85" s="7">
         <v>13.8289529548574</v>
       </c>
-      <c r="F85" s="8">
+      <c r="F85" s="7">
         <v>13.290458919063401</v>
       </c>
-      <c r="G85" s="8">
+      <c r="G85" s="7">
         <v>13.7984963244865</v>
       </c>
       <c r="H85">
@@ -11329,22 +11329,22 @@
       <c r="I85" s="1"/>
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B86" s="8">
+      <c r="B86" s="7">
         <v>2020</v>
       </c>
-      <c r="C86" s="8" t="s">
+      <c r="C86" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D86" s="8">
+      <c r="D86" s="7">
         <v>0.122414483903036</v>
       </c>
-      <c r="E86" s="8">
+      <c r="E86" s="7">
         <v>2.6011623535777302</v>
       </c>
-      <c r="F86" s="8">
+      <c r="F86" s="7">
         <v>0.79932670257081995</v>
       </c>
-      <c r="G86" s="8">
+      <c r="G86" s="7">
         <v>3.8651403135274198</v>
       </c>
       <c r="H86">
@@ -11354,22 +11354,22 @@
       <c r="I86" s="1"/>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B87" s="8">
+      <c r="B87" s="7">
         <v>2020</v>
       </c>
-      <c r="C87" s="8" t="s">
+      <c r="C87" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D87" s="8">
+      <c r="D87" s="7">
         <v>13.099440837606901</v>
       </c>
-      <c r="E87" s="8">
+      <c r="E87" s="7">
         <v>10.934820189219399</v>
       </c>
-      <c r="F87" s="8">
+      <c r="F87" s="7">
         <v>17.7464621349087</v>
       </c>
-      <c r="G87" s="8">
+      <c r="G87" s="7">
         <v>43.900893795354598</v>
       </c>
       <c r="H87">
@@ -11379,20 +11379,20 @@
       <c r="I87" s="1"/>
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B88" s="8">
+      <c r="B88" s="7">
         <v>2020</v>
       </c>
-      <c r="C88" s="8" t="s">
+      <c r="C88" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D88" s="8"/>
-      <c r="E88" s="8">
+      <c r="D88" s="7"/>
+      <c r="E88" s="7">
         <v>43.973106127371899</v>
       </c>
-      <c r="F88" s="8">
+      <c r="F88" s="7">
         <v>35.645068774391298</v>
       </c>
-      <c r="G88" s="8">
+      <c r="G88" s="7">
         <v>71.021737625213802</v>
       </c>
       <c r="H88">
@@ -11402,22 +11402,22 @@
       <c r="I88" s="1"/>
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B89" s="8">
+      <c r="B89" s="7">
         <v>2020</v>
       </c>
-      <c r="C89" s="8" t="s">
+      <c r="C89" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D89" s="8">
+      <c r="D89" s="7">
         <v>12.097771601517399</v>
       </c>
-      <c r="E89" s="8">
+      <c r="E89" s="7">
         <v>12.6382691817671</v>
       </c>
-      <c r="F89" s="8">
+      <c r="F89" s="7">
         <v>23.4217080481449</v>
       </c>
-      <c r="G89" s="8">
+      <c r="G89" s="7">
         <v>6.9597791903529203</v>
       </c>
       <c r="H89">
@@ -11427,22 +11427,22 @@
       <c r="I89" s="1"/>
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B90" s="8">
+      <c r="B90" s="7">
         <v>2020</v>
       </c>
-      <c r="C90" s="8" t="s">
+      <c r="C90" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D90" s="8">
+      <c r="D90" s="7">
         <v>3.8008194469150198</v>
       </c>
-      <c r="E90" s="8">
+      <c r="E90" s="7">
         <v>5.8004991814476199</v>
       </c>
-      <c r="F90" s="8">
+      <c r="F90" s="7">
         <v>16.002335279716501</v>
       </c>
-      <c r="G90" s="8">
+      <c r="G90" s="7">
         <v>15.0077097128835</v>
       </c>
       <c r="H90">
@@ -11452,22 +11452,22 @@
       <c r="I90" s="1"/>
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B91" s="8">
+      <c r="B91" s="7">
         <v>2020</v>
       </c>
-      <c r="C91" s="8" t="s">
+      <c r="C91" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D91" s="8">
+      <c r="D91" s="7">
         <v>3.5721419532649699</v>
       </c>
-      <c r="E91" s="8">
+      <c r="E91" s="7">
         <v>4.0653535115755099</v>
       </c>
-      <c r="F91" s="8">
+      <c r="F91" s="7">
         <v>13.450798176825201</v>
       </c>
-      <c r="G91" s="8">
+      <c r="G91" s="7">
         <v>48.1550496959673</v>
       </c>
       <c r="H91">
@@ -11477,22 +11477,22 @@
       <c r="I91" s="1"/>
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B92" s="8">
+      <c r="B92" s="7">
         <v>2020</v>
       </c>
-      <c r="C92" s="8" t="s">
+      <c r="C92" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D92" s="8">
+      <c r="D92" s="7">
         <v>5.7803921420397399</v>
       </c>
-      <c r="E92" s="8">
+      <c r="E92" s="7">
         <v>6.4621356695688101</v>
       </c>
-      <c r="F92" s="8">
+      <c r="F92" s="7">
         <v>8.1558779939742703</v>
       </c>
-      <c r="G92" s="8">
+      <c r="G92" s="7">
         <v>8.89382407968127</v>
       </c>
       <c r="H92">
@@ -11502,22 +11502,22 @@
       <c r="I92" s="1"/>
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B93" s="8">
+      <c r="B93" s="7">
         <v>2020</v>
       </c>
-      <c r="C93" s="8" t="s">
+      <c r="C93" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D93" s="8">
+      <c r="D93" s="7">
         <v>278.82689497737198</v>
       </c>
-      <c r="E93" s="8">
+      <c r="E93" s="7">
         <v>351.21587179083502</v>
       </c>
-      <c r="F93" s="8">
+      <c r="F93" s="7">
         <v>424.842699575214</v>
       </c>
-      <c r="G93" s="8">
+      <c r="G93" s="7">
         <v>302.50094955740798</v>
       </c>
       <c r="H93">
@@ -11527,22 +11527,22 @@
       <c r="I93" s="1"/>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B94" s="8">
+      <c r="B94" s="7">
         <v>2020</v>
       </c>
-      <c r="C94" s="8" t="s">
+      <c r="C94" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D94" s="8">
+      <c r="D94" s="7">
         <v>302.82538954331102</v>
       </c>
-      <c r="E94" s="8">
+      <c r="E94" s="7">
         <v>525.01728569190095</v>
       </c>
-      <c r="F94" s="8">
+      <c r="F94" s="7">
         <v>972.74355424747603</v>
       </c>
-      <c r="G94" s="8">
+      <c r="G94" s="7">
         <v>793.48940365759597</v>
       </c>
       <c r="H94">
@@ -11552,22 +11552,22 @@
       <c r="I94" s="1"/>
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B95" s="8">
+      <c r="B95" s="7">
         <v>2020</v>
       </c>
-      <c r="C95" s="8" t="s">
+      <c r="C95" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D95" s="8">
+      <c r="D95" s="7">
         <v>40.005651658170798</v>
       </c>
-      <c r="E95" s="8">
+      <c r="E95" s="7">
         <v>97.875458788018904</v>
       </c>
-      <c r="F95" s="8">
+      <c r="F95" s="7">
         <v>242.57663778521399</v>
       </c>
-      <c r="G95" s="8">
+      <c r="G95" s="7">
         <v>182.09495513784401</v>
       </c>
       <c r="H95">
@@ -11577,22 +11577,22 @@
       <c r="I95" s="1"/>
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B96" s="8">
+      <c r="B96" s="7">
         <v>2020</v>
       </c>
-      <c r="C96" s="8" t="s">
+      <c r="C96" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D96" s="8">
+      <c r="D96" s="7">
         <v>3.5454575233041199</v>
       </c>
-      <c r="E96" s="8">
+      <c r="E96" s="7">
         <v>6.5637649283364699</v>
       </c>
-      <c r="F96" s="8">
+      <c r="F96" s="7">
         <v>21.391075882591299</v>
       </c>
-      <c r="G96" s="8">
+      <c r="G96" s="7">
         <v>25.6363987377256</v>
       </c>
       <c r="H96">
@@ -11602,22 +11602,22 @@
       <c r="I96" s="1"/>
     </row>
     <row r="97" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B97" s="8">
+      <c r="B97" s="7">
         <v>2020</v>
       </c>
-      <c r="C97" s="8" t="s">
+      <c r="C97" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D97" s="8">
+      <c r="D97" s="7">
         <v>7.8393519960124998</v>
       </c>
-      <c r="E97" s="8">
+      <c r="E97" s="7">
         <v>15.4653343989487</v>
       </c>
-      <c r="F97" s="8">
+      <c r="F97" s="7">
         <v>16.949095913197301</v>
       </c>
-      <c r="G97" s="8">
+      <c r="G97" s="7">
         <v>9.2046628426968393</v>
       </c>
       <c r="H97">
@@ -11627,22 +11627,22 @@
       <c r="I97" s="1"/>
     </row>
     <row r="98" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B98" s="8">
+      <c r="B98" s="7">
         <v>2020</v>
       </c>
-      <c r="C98" s="8" t="s">
+      <c r="C98" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D98" s="8">
+      <c r="D98" s="7">
         <v>33.542115724270403</v>
       </c>
-      <c r="E98" s="8">
+      <c r="E98" s="7">
         <v>66.171290227548994</v>
       </c>
-      <c r="F98" s="8">
+      <c r="F98" s="7">
         <v>72.519837970204406</v>
       </c>
-      <c r="G98" s="8">
+      <c r="G98" s="7">
         <v>39.383850403664802</v>
       </c>
       <c r="H98">
@@ -11652,20 +11652,20 @@
       <c r="I98" s="1"/>
     </row>
     <row r="99" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B99" s="8">
+      <c r="B99" s="7">
         <v>2020</v>
       </c>
-      <c r="C99" s="8" t="s">
+      <c r="C99" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D99" s="8"/>
-      <c r="E99" s="8">
+      <c r="D99" s="7"/>
+      <c r="E99" s="7">
         <v>5.8434840725380202E-4</v>
       </c>
-      <c r="F99" s="8">
+      <c r="F99" s="7">
         <v>8.8053936827785104E-2</v>
       </c>
-      <c r="G99" s="8">
+      <c r="G99" s="7">
         <v>7.3890767209723193E-2</v>
       </c>
       <c r="H99">
@@ -11675,22 +11675,22 @@
       <c r="I99" s="1"/>
     </row>
     <row r="100" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B100" s="8">
+      <c r="B100" s="7">
         <v>2020</v>
       </c>
-      <c r="C100" s="8" t="s">
+      <c r="C100" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D100" s="8">
+      <c r="D100" s="7">
         <v>0.54599352264248102</v>
       </c>
-      <c r="E100" s="8">
+      <c r="E100" s="7">
         <v>0.38923325387254198</v>
       </c>
-      <c r="F100" s="8">
+      <c r="F100" s="7">
         <v>2.7845008598685901</v>
       </c>
-      <c r="G100" s="8">
+      <c r="G100" s="7">
         <v>4.6389784384911001</v>
       </c>
       <c r="H100">
@@ -11700,22 +11700,22 @@
       <c r="I100" s="1"/>
     </row>
     <row r="101" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B101" s="8">
+      <c r="B101" s="7">
         <v>2020</v>
       </c>
-      <c r="C101" s="8" t="s">
+      <c r="C101" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D101" s="8">
+      <c r="D101" s="7">
         <v>3.1026797551499801</v>
       </c>
-      <c r="E101" s="8">
+      <c r="E101" s="7">
         <v>12.966990044156899</v>
       </c>
-      <c r="F101" s="8">
+      <c r="F101" s="7">
         <v>49.194044909657599</v>
       </c>
-      <c r="G101" s="8">
+      <c r="G101" s="7">
         <v>87.441716265859597</v>
       </c>
       <c r="H101">
@@ -11725,22 +11725,22 @@
       <c r="I101" s="1"/>
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B102" s="8">
+      <c r="B102" s="7">
         <v>2020</v>
       </c>
-      <c r="C102" s="8" t="s">
+      <c r="C102" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D102" s="8">
+      <c r="D102" s="7">
         <v>3.9903442558872002</v>
       </c>
-      <c r="E102" s="8">
+      <c r="E102" s="7">
         <v>4.4360182726249997</v>
       </c>
-      <c r="F102" s="8">
+      <c r="F102" s="7">
         <v>90.021348044644398</v>
       </c>
-      <c r="G102" s="8">
+      <c r="G102" s="7">
         <v>226.74332250322101</v>
       </c>
       <c r="H102">
@@ -11750,22 +11750,22 @@
       <c r="I102" s="1"/>
     </row>
     <row r="103" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B103" s="8">
+      <c r="B103" s="7">
         <v>2020</v>
       </c>
-      <c r="C103" s="8" t="s">
+      <c r="C103" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D103" s="8">
+      <c r="D103" s="7">
         <v>59.551402044539998</v>
       </c>
-      <c r="E103" s="8">
+      <c r="E103" s="7">
         <v>162.43230438484301</v>
       </c>
-      <c r="F103" s="8">
+      <c r="F103" s="7">
         <v>441.92728348383798</v>
       </c>
-      <c r="G103" s="8">
+      <c r="G103" s="7">
         <v>533.90532520061595</v>
       </c>
       <c r="H103">
@@ -11775,22 +11775,22 @@
       <c r="I103" s="1"/>
     </row>
     <row r="104" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B104" s="8">
+      <c r="B104" s="7">
         <v>2020</v>
       </c>
-      <c r="C104" s="8" t="s">
+      <c r="C104" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D104" s="8">
+      <c r="D104" s="7">
         <v>40.3836291681137</v>
       </c>
-      <c r="E104" s="8">
+      <c r="E104" s="7">
         <v>78.585234333748005</v>
       </c>
-      <c r="F104" s="8">
+      <c r="F104" s="7">
         <v>243.012242689018</v>
       </c>
-      <c r="G104" s="8">
+      <c r="G104" s="7">
         <v>543.41397738827004</v>
       </c>
       <c r="H104">
@@ -11800,22 +11800,22 @@
       <c r="I104" s="1"/>
     </row>
     <row r="105" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B105" s="8">
+      <c r="B105" s="7">
         <v>2020</v>
       </c>
-      <c r="C105" s="8" t="s">
+      <c r="C105" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D105" s="8">
+      <c r="D105" s="7">
         <v>876.87025097256299</v>
       </c>
-      <c r="E105" s="8">
+      <c r="E105" s="7">
         <v>1081.30768531237</v>
       </c>
-      <c r="F105" s="8">
+      <c r="F105" s="7">
         <v>781.96521805462805</v>
       </c>
-      <c r="G105" s="8">
+      <c r="G105" s="7">
         <v>1365.6124247047301</v>
       </c>
       <c r="H105">
@@ -11825,22 +11825,22 @@
       <c r="I105" s="1"/>
     </row>
     <row r="106" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B106" s="8">
+      <c r="B106" s="7">
         <v>2020</v>
       </c>
-      <c r="C106" s="8" t="s">
+      <c r="C106" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D106" s="9">
+      <c r="D106" s="8">
         <v>4.1489673071146102E-9</v>
       </c>
-      <c r="E106" s="9">
+      <c r="E106" s="8">
         <v>2.1887416944773499E-9</v>
       </c>
-      <c r="F106" s="9">
+      <c r="F106" s="8">
         <v>1.45976889111928E-9</v>
       </c>
-      <c r="G106" s="9">
+      <c r="G106" s="8">
         <v>8.1017229330277199E-10</v>
       </c>
       <c r="H106">
@@ -11909,7 +11909,7 @@
         <v>2</v>
       </c>
       <c r="Z1">
-        <f t="shared" ref="Z1:AX1" si="1">U1+1</f>
+        <f t="shared" ref="Z1:AW1" si="1">U1+1</f>
         <v>2</v>
       </c>
       <c r="AA1">
@@ -22948,14 +22948,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D099A1C4-AB42-452C-A882-EFEEEDB6173D}">
   <dimension ref="A1:AM27"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="AN4" sqref="AN4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" customWidth="1"/>
     <col min="3" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.28515625" bestFit="1" customWidth="1"/>
@@ -22995,33 +22995,33 @@
       </c>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.2">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="K2" s="5" t="s">
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="K2" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="T2" s="5" t="s">
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="T2" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
-      <c r="W2" s="5"/>
-      <c r="X2" s="5"/>
-      <c r="Y2" s="5"/>
-      <c r="Z2" s="5"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="9"/>
+      <c r="W2" s="9"/>
+      <c r="X2" s="9"/>
+      <c r="Y2" s="9"/>
+      <c r="Z2" s="9"/>
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.2">
       <c r="B3">
@@ -23202,27 +23202,27 @@
         <v>-0.19445579545170144</v>
       </c>
       <c r="U4" s="3">
-        <f t="shared" ref="U4:U24" si="2">C4-L4</f>
+        <f t="shared" ref="U4:U18" si="2">C4-L4</f>
         <v>2.5243232988029163E-2</v>
       </c>
       <c r="V4" s="3">
-        <f t="shared" ref="V4:V24" si="3">D4-M4</f>
+        <f t="shared" ref="V4:V18" si="3">D4-M4</f>
         <v>0.1408802792845405</v>
       </c>
       <c r="W4" s="3">
-        <f t="shared" ref="W4:W24" si="4">E4-N4</f>
+        <f t="shared" ref="W4:W18" si="4">E4-N4</f>
         <v>0.16229147533961763</v>
       </c>
       <c r="X4" s="3">
-        <f t="shared" ref="X4:X24" si="5">F4-O4</f>
+        <f t="shared" ref="X4:X18" si="5">F4-O4</f>
         <v>0.27723079236947878</v>
       </c>
       <c r="Y4" s="3">
-        <f t="shared" ref="Y4:Y24" si="6">G4-P4</f>
+        <f t="shared" ref="Y4:Y18" si="6">G4-P4</f>
         <v>0.12641070394222176</v>
       </c>
       <c r="Z4" s="3">
-        <f t="shared" ref="Z4:Z24" si="7">H4-Q4</f>
+        <f t="shared" ref="Z4:Z18" si="7">H4-Q4</f>
         <v>5.4078028330307504E-2</v>
       </c>
       <c r="AB4" t="s">
@@ -23340,7 +23340,7 @@
         <v>57</v>
       </c>
       <c r="T5" s="3">
-        <f t="shared" ref="T5:T24" si="8">B5-K5</f>
+        <f t="shared" ref="T5:T18" si="8">B5-K5</f>
         <v>-0.73072355342783979</v>
       </c>
       <c r="U5" s="3">
@@ -23645,952 +23645,952 @@
         <v>-0.46460034282159501</v>
       </c>
     </row>
-    <row r="8" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:39" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="6">
         <f>VLOOKUP($A8,Sheet2!$A$3:$H$74,B$1,)</f>
         <v>-5.0389999999999997</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="6">
         <f>VLOOKUP($A8,Sheet2!$A$3:$H$74,C$1,)</f>
         <v>0.94399999999999995</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="6">
         <f>VLOOKUP($A8,Sheet2!$A$3:$H$74,D$1,)</f>
         <v>2.4319999999999999</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="6">
         <f>VLOOKUP($A8,Sheet2!$A$3:$H$74,E$1,)</f>
         <v>2.1585999999999999</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="6">
         <f>VLOOKUP($A8,Sheet2!$A$3:$H$74,F$1,)</f>
         <v>2.3109999999999999</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="6">
         <f>VLOOKUP($A8,Sheet2!$A$3:$H$74,G$1,)</f>
         <v>2.1974</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="6">
         <f>VLOOKUP($A8,Sheet2!$A$3:$H$74,H$1,)</f>
         <v>2.3693333333333331</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J8" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="K8" s="7">
+      <c r="K8" s="6">
         <f>[1]ManSUTdet!U41*100</f>
         <v>-8.3692583620596004</v>
       </c>
-      <c r="L8" s="7">
+      <c r="L8" s="6">
         <f>[1]ManSUTdet!BC41*100</f>
         <v>0.52614832758807983</v>
       </c>
-      <c r="M8" s="7">
+      <c r="M8" s="6">
         <f>[1]ManSUTdet!BD41*100</f>
         <v>2.8200000000000003</v>
       </c>
-      <c r="N8" s="7">
+      <c r="N8" s="6">
         <f>[1]ManSUTdet!BE41*100</f>
         <v>2.98</v>
       </c>
-      <c r="O8" s="7">
+      <c r="O8" s="6">
         <f>[1]ManSUTdet!BF41*100</f>
         <v>3.2399999999999998</v>
       </c>
-      <c r="P8" s="7">
+      <c r="P8" s="6">
         <f>[1]ManSUTdet!BG41*100</f>
         <v>3.4600000000000004</v>
       </c>
-      <c r="Q8" s="7">
+      <c r="Q8" s="6">
         <f>[1]ManSUTdet!BH41*100</f>
         <v>3.6666666666666674</v>
       </c>
-      <c r="S8" s="6" t="s">
+      <c r="S8" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="T8" s="7">
+      <c r="T8" s="6">
         <f t="shared" si="8"/>
         <v>3.3302583620596007</v>
       </c>
-      <c r="U8" s="7">
+      <c r="U8" s="6">
         <f t="shared" si="2"/>
         <v>0.41785167241192012</v>
       </c>
-      <c r="V8" s="7">
+      <c r="V8" s="6">
         <f t="shared" si="3"/>
         <v>-0.38800000000000034</v>
       </c>
-      <c r="W8" s="7">
+      <c r="W8" s="6">
         <f t="shared" si="4"/>
         <v>-0.82140000000000013</v>
       </c>
-      <c r="X8" s="7">
+      <c r="X8" s="6">
         <f t="shared" si="5"/>
         <v>-0.92899999999999983</v>
       </c>
-      <c r="Y8" s="7">
+      <c r="Y8" s="6">
         <f t="shared" si="6"/>
         <v>-1.2626000000000004</v>
       </c>
-      <c r="Z8" s="7">
+      <c r="Z8" s="6">
         <f t="shared" si="7"/>
         <v>-1.2973333333333343</v>
       </c>
     </row>
-    <row r="9" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:39" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <f>VLOOKUP($A9,Sheet2!$A$3:$H$74,B$1,)</f>
         <v>-9.6859999999999999</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <f>VLOOKUP($A9,Sheet2!$A$3:$H$74,C$1,)</f>
         <v>9.3599999999999989E-2</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="6">
         <f>VLOOKUP($A9,Sheet2!$A$3:$H$74,D$1,)</f>
         <v>2.7423999999999999</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="6">
         <f>VLOOKUP($A9,Sheet2!$A$3:$H$74,E$1,)</f>
         <v>2.4964000000000004</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="6">
         <f>VLOOKUP($A9,Sheet2!$A$3:$H$74,F$1,)</f>
         <v>2.6120000000000001</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="6">
         <f>VLOOKUP($A9,Sheet2!$A$3:$H$74,G$1,)</f>
         <v>2.5542000000000002</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="6">
         <f>VLOOKUP($A9,Sheet2!$A$3:$H$74,H$1,)</f>
         <v>2.7906666666666666</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="J9" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="K9" s="7">
+      <c r="K9" s="6">
         <f>[1]ManSUTdet!U42*100</f>
         <v>-19.186539748694077</v>
       </c>
-      <c r="L9" s="7">
+      <c r="L9" s="6">
         <f>[1]ManSUTdet!BC42*100</f>
         <v>-2.177307949738815</v>
       </c>
-      <c r="M9" s="7">
+      <c r="M9" s="6">
         <f>[1]ManSUTdet!BD42*100</f>
         <v>2.4</v>
       </c>
-      <c r="N9" s="7">
+      <c r="N9" s="6">
         <f>[1]ManSUTdet!BE42*100</f>
         <v>2.66</v>
       </c>
-      <c r="O9" s="7">
+      <c r="O9" s="6">
         <f>[1]ManSUTdet!BF42*100</f>
         <v>2.94</v>
       </c>
-      <c r="P9" s="7">
+      <c r="P9" s="6">
         <f>[1]ManSUTdet!BG42*100</f>
         <v>3.2399999999999998</v>
       </c>
-      <c r="Q9" s="7">
+      <c r="Q9" s="6">
         <f>[1]ManSUTdet!BH42*100</f>
         <v>3.4666666666666672</v>
       </c>
-      <c r="S9" s="6" t="s">
+      <c r="S9" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="T9" s="7">
+      <c r="T9" s="6">
         <f t="shared" si="8"/>
         <v>9.5005397486940772</v>
       </c>
-      <c r="U9" s="7">
+      <c r="U9" s="6">
         <f t="shared" si="2"/>
         <v>2.2709079497388149</v>
       </c>
-      <c r="V9" s="7">
+      <c r="V9" s="6">
         <f t="shared" si="3"/>
         <v>0.34240000000000004</v>
       </c>
-      <c r="W9" s="7">
+      <c r="W9" s="6">
         <f t="shared" si="4"/>
         <v>-0.16359999999999975</v>
       </c>
-      <c r="X9" s="7">
+      <c r="X9" s="6">
         <f t="shared" si="5"/>
         <v>-0.32799999999999985</v>
       </c>
-      <c r="Y9" s="7">
+      <c r="Y9" s="6">
         <f t="shared" si="6"/>
         <v>-0.68579999999999952</v>
       </c>
-      <c r="Z9" s="7">
+      <c r="Z9" s="6">
         <f t="shared" si="7"/>
         <v>-0.6760000000000006</v>
       </c>
     </row>
-    <row r="10" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+    <row r="10" spans="1:39" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="6">
         <f>VLOOKUP($A10,Sheet2!$A$3:$H$74,B$1,)</f>
         <v>-7.4359999999999999</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="6">
         <f>VLOOKUP($A10,Sheet2!$A$3:$H$74,C$1,)</f>
         <v>0.42599999999999999</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="6">
         <f>VLOOKUP($A10,Sheet2!$A$3:$H$74,D$1,)</f>
         <v>2.5534000000000003</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="6">
         <f>VLOOKUP($A10,Sheet2!$A$3:$H$74,E$1,)</f>
         <v>2.6459999999999999</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="6">
         <f>VLOOKUP($A10,Sheet2!$A$3:$H$74,F$1,)</f>
         <v>2.9474000000000005</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="6">
         <f>VLOOKUP($A10,Sheet2!$A$3:$H$74,G$1,)</f>
         <v>3.0318000000000001</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="6">
         <f>VLOOKUP($A10,Sheet2!$A$3:$H$74,H$1,)</f>
         <v>3.2678333333333334</v>
       </c>
-      <c r="J10" s="6" t="s">
+      <c r="J10" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="K10" s="7">
+      <c r="K10" s="6">
         <f>[1]ManSUTdet!U43*100</f>
         <v>-15.007712627548402</v>
       </c>
-      <c r="L10" s="7">
+      <c r="L10" s="6">
         <f>[1]ManSUTdet!BC43*100</f>
         <v>-0.94154252550968043</v>
       </c>
-      <c r="M10" s="7">
+      <c r="M10" s="6">
         <f>[1]ManSUTdet!BD43*100</f>
         <v>2.46</v>
       </c>
-      <c r="N10" s="7">
+      <c r="N10" s="6">
         <f>[1]ManSUTdet!BE43*100</f>
         <v>2.5</v>
       </c>
-      <c r="O10" s="7">
+      <c r="O10" s="6">
         <f>[1]ManSUTdet!BF43*100</f>
         <v>2.66</v>
       </c>
-      <c r="P10" s="7">
+      <c r="P10" s="6">
         <f>[1]ManSUTdet!BG43*100</f>
         <v>2.7800000000000002</v>
       </c>
-      <c r="Q10" s="7">
+      <c r="Q10" s="6">
         <f>[1]ManSUTdet!BH43*100</f>
         <v>2.8000000000000003</v>
       </c>
-      <c r="S10" s="6" t="s">
+      <c r="S10" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="T10" s="7">
+      <c r="T10" s="6">
         <f t="shared" si="8"/>
         <v>7.5717126275484024</v>
       </c>
-      <c r="U10" s="7">
+      <c r="U10" s="6">
         <f t="shared" si="2"/>
         <v>1.3675425255096805</v>
       </c>
-      <c r="V10" s="7">
+      <c r="V10" s="6">
         <f t="shared" si="3"/>
         <v>9.3400000000000372E-2</v>
       </c>
-      <c r="W10" s="7">
+      <c r="W10" s="6">
         <f t="shared" si="4"/>
         <v>0.14599999999999991</v>
       </c>
-      <c r="X10" s="7">
+      <c r="X10" s="6">
         <f t="shared" si="5"/>
         <v>0.28740000000000032</v>
       </c>
-      <c r="Y10" s="7">
+      <c r="Y10" s="6">
         <f t="shared" si="6"/>
         <v>0.2517999999999998</v>
       </c>
-      <c r="Z10" s="7">
+      <c r="Z10" s="6">
         <f t="shared" si="7"/>
         <v>0.4678333333333331</v>
       </c>
     </row>
-    <row r="11" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+    <row r="11" spans="1:39" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="6">
         <f>VLOOKUP($A11,Sheet2!$A$3:$H$74,B$1,)</f>
         <v>-0.29799999999999999</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6">
         <f>VLOOKUP($A11,Sheet2!$A$3:$H$74,C$1,)</f>
         <v>-1.2088000000000001</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="6">
         <f>VLOOKUP($A11,Sheet2!$A$3:$H$74,D$1,)</f>
         <v>-9.3201999999999998</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="6">
         <f>VLOOKUP($A11,Sheet2!$A$3:$H$74,E$1,)</f>
         <v>-9.7330000000000005</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="6">
         <f>VLOOKUP($A11,Sheet2!$A$3:$H$74,F$1,)</f>
         <v>-16.8048</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="6">
         <f>VLOOKUP($A11,Sheet2!$A$3:$H$74,G$1,)</f>
         <v>-6.3628</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="6">
         <f>VLOOKUP($A11,Sheet2!$A$3:$H$74,H$1,)</f>
         <v>0</v>
       </c>
-      <c r="J11" s="6" t="s">
+      <c r="J11" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K11" s="7">
+      <c r="K11" s="6">
         <f>[1]ManSUTdet!U44*100</f>
         <v>-0.3</v>
       </c>
-      <c r="L11" s="7">
+      <c r="L11" s="6">
         <f>[1]ManSUTdet!BC44*100</f>
         <v>-1.244</v>
       </c>
-      <c r="M11" s="7">
+      <c r="M11" s="6">
         <f>[1]ManSUTdet!BD44*100</f>
         <v>-9.5780000000000012</v>
       </c>
-      <c r="N11" s="7">
+      <c r="N11" s="6">
         <f>[1]ManSUTdet!BE44*100</f>
         <v>-10.098000000000001</v>
       </c>
-      <c r="O11" s="7">
+      <c r="O11" s="6">
         <f>[1]ManSUTdet!BF44*100</f>
         <v>-16.343999999999998</v>
       </c>
-      <c r="P11" s="7">
+      <c r="P11" s="6">
         <f>[1]ManSUTdet!BG44*100</f>
         <v>-5.976</v>
       </c>
-      <c r="Q11" s="7">
+      <c r="Q11" s="6">
         <f>[1]ManSUTdet!BH44*100</f>
         <v>0</v>
       </c>
-      <c r="S11" s="6" t="s">
+      <c r="S11" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="T11" s="7">
+      <c r="T11" s="6">
         <f t="shared" si="8"/>
         <v>2.0000000000000018E-3</v>
       </c>
-      <c r="U11" s="7">
+      <c r="U11" s="6">
         <f t="shared" si="2"/>
         <v>3.5199999999999898E-2</v>
       </c>
-      <c r="V11" s="7">
+      <c r="V11" s="6">
         <f t="shared" si="3"/>
         <v>0.25780000000000136</v>
       </c>
-      <c r="W11" s="7">
+      <c r="W11" s="6">
         <f t="shared" si="4"/>
         <v>0.36500000000000021</v>
       </c>
-      <c r="X11" s="7">
+      <c r="X11" s="6">
         <f t="shared" si="5"/>
         <v>-0.46080000000000254</v>
       </c>
-      <c r="Y11" s="7">
+      <c r="Y11" s="6">
         <f t="shared" si="6"/>
         <v>-0.38680000000000003</v>
       </c>
-      <c r="Z11" s="7">
+      <c r="Z11" s="6">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+    <row r="12" spans="1:39" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="6">
         <f>VLOOKUP($A12,Sheet2!$A$3:$H$74,B$1,)</f>
         <v>-8.0519999999999996</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="6">
         <f>VLOOKUP($A12,Sheet2!$A$3:$H$74,C$1,)</f>
         <v>0.22780000000000006</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="6">
         <f>VLOOKUP($A12,Sheet2!$A$3:$H$74,D$1,)</f>
         <v>2.7643999999999997</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="6">
         <f>VLOOKUP($A12,Sheet2!$A$3:$H$74,E$1,)</f>
         <v>3.4843999999999999</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="6">
         <f>VLOOKUP($A12,Sheet2!$A$3:$H$74,F$1,)</f>
         <v>3.6327999999999996</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="6">
         <f>VLOOKUP($A12,Sheet2!$A$3:$H$74,G$1,)</f>
         <v>3.3334000000000001</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="6">
         <f>VLOOKUP($A12,Sheet2!$A$3:$H$74,H$1,)</f>
         <v>3.2501666666666669</v>
       </c>
-      <c r="J12" s="6" t="s">
+      <c r="J12" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K12" s="6">
         <f>[1]ManSUTdet!U45*100</f>
         <v>-6.3955132495646909</v>
       </c>
-      <c r="L12" s="7">
+      <c r="L12" s="6">
         <f>[1]ManSUTdet!BC45*100</f>
         <v>0.58089735008706178</v>
       </c>
-      <c r="M12" s="7">
+      <c r="M12" s="6">
         <f>[1]ManSUTdet!BD45*100</f>
         <v>2.1999999999999997</v>
       </c>
-      <c r="N12" s="7">
+      <c r="N12" s="6">
         <f>[1]ManSUTdet!BE45*100</f>
         <v>2.2999999999999998</v>
       </c>
-      <c r="O12" s="7">
+      <c r="O12" s="6">
         <f>[1]ManSUTdet!BF45*100</f>
         <v>2.46</v>
       </c>
-      <c r="P12" s="7">
+      <c r="P12" s="6">
         <f>[1]ManSUTdet!BG45*100</f>
         <v>2.9</v>
       </c>
-      <c r="Q12" s="7">
+      <c r="Q12" s="6">
         <f>[1]ManSUTdet!BH45*100</f>
         <v>3.25</v>
       </c>
-      <c r="S12" s="6" t="s">
+      <c r="S12" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="T12" s="7">
+      <c r="T12" s="6">
         <f t="shared" si="8"/>
         <v>-1.6564867504353087</v>
       </c>
-      <c r="U12" s="7">
+      <c r="U12" s="6">
         <f t="shared" si="2"/>
         <v>-0.35309735008706172</v>
       </c>
-      <c r="V12" s="7">
+      <c r="V12" s="6">
         <f t="shared" si="3"/>
         <v>0.56440000000000001</v>
       </c>
-      <c r="W12" s="7">
+      <c r="W12" s="6">
         <f t="shared" si="4"/>
         <v>1.1844000000000001</v>
       </c>
-      <c r="X12" s="7">
+      <c r="X12" s="6">
         <f t="shared" si="5"/>
         <v>1.1727999999999996</v>
       </c>
-      <c r="Y12" s="7">
+      <c r="Y12" s="6">
         <f t="shared" si="6"/>
         <v>0.43340000000000023</v>
       </c>
-      <c r="Z12" s="7">
+      <c r="Z12" s="6">
         <f t="shared" si="7"/>
         <v>1.6666666666687036E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+    <row r="13" spans="1:39" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="6">
         <f>VLOOKUP($A13,Sheet2!$A$3:$H$74,B$1,)</f>
         <v>-8.5359999999999996</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="6">
         <f>VLOOKUP($A13,Sheet2!$A$3:$H$74,C$1,)</f>
         <v>0.22760000000000008</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="6">
         <f>VLOOKUP($A13,Sheet2!$A$3:$H$74,D$1,)</f>
         <v>2.62</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="6">
         <f>VLOOKUP($A13,Sheet2!$A$3:$H$74,E$1,)</f>
         <v>2.8595999999999999</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="6">
         <f>VLOOKUP($A13,Sheet2!$A$3:$H$74,F$1,)</f>
         <v>3.1383999999999999</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="6">
         <f>VLOOKUP($A13,Sheet2!$A$3:$H$74,G$1,)</f>
         <v>3.2316000000000003</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H13" s="6">
         <f>VLOOKUP($A13,Sheet2!$A$3:$H$74,H$1,)</f>
         <v>3.4863333333333331</v>
       </c>
-      <c r="J13" s="6" t="s">
+      <c r="J13" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="K13" s="7">
+      <c r="K13" s="6">
         <f>[1]ManSUTdet!U46*100</f>
         <v>-12.791026499129382</v>
       </c>
-      <c r="L13" s="7">
+      <c r="L13" s="6">
         <f>[1]ManSUTdet!BC46*100</f>
         <v>-7.8205299825876359E-2</v>
       </c>
-      <c r="M13" s="7">
+      <c r="M13" s="6">
         <f>[1]ManSUTdet!BD46*100</f>
         <v>2.7</v>
       </c>
-      <c r="N13" s="7">
+      <c r="N13" s="6">
         <f>[1]ManSUTdet!BE46*100</f>
         <v>2.8000000000000003</v>
       </c>
-      <c r="O13" s="7">
+      <c r="O13" s="6">
         <f>[1]ManSUTdet!BF46*100</f>
         <v>2.96</v>
       </c>
-      <c r="P13" s="7">
+      <c r="P13" s="6">
         <f>[1]ManSUTdet!BG46*100</f>
         <v>3.2399999999999998</v>
       </c>
-      <c r="Q13" s="7">
+      <c r="Q13" s="6">
         <f>[1]ManSUTdet!BH46*100</f>
         <v>3.4666666666666672</v>
       </c>
-      <c r="S13" s="6" t="s">
+      <c r="S13" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="T13" s="7">
+      <c r="T13" s="6">
         <f t="shared" si="8"/>
         <v>4.2550264991293822</v>
       </c>
-      <c r="U13" s="7">
+      <c r="U13" s="6">
         <f t="shared" si="2"/>
         <v>0.30580529982587645</v>
       </c>
-      <c r="V13" s="7">
+      <c r="V13" s="6">
         <f t="shared" si="3"/>
         <v>-8.0000000000000071E-2</v>
       </c>
-      <c r="W13" s="7">
+      <c r="W13" s="6">
         <f t="shared" si="4"/>
         <v>5.9599999999999653E-2</v>
       </c>
-      <c r="X13" s="7">
+      <c r="X13" s="6">
         <f t="shared" si="5"/>
         <v>0.17839999999999989</v>
       </c>
-      <c r="Y13" s="7">
+      <c r="Y13" s="6">
         <f t="shared" si="6"/>
         <v>-8.399999999999519E-3</v>
       </c>
-      <c r="Z13" s="7">
+      <c r="Z13" s="6">
         <f t="shared" si="7"/>
         <v>1.9666666666665833E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:39" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="6">
         <f>VLOOKUP($A14,Sheet2!$A$3:$H$74,B$1,)</f>
         <v>-11.914</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="6">
         <f>VLOOKUP($A14,Sheet2!$A$3:$H$74,C$1,)</f>
         <v>-0.66079999999999983</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="6">
         <f>VLOOKUP($A14,Sheet2!$A$3:$H$74,D$1,)</f>
         <v>2.7658</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="6">
         <f>VLOOKUP($A14,Sheet2!$A$3:$H$74,E$1,)</f>
         <v>2.6003999999999996</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="6">
         <f>VLOOKUP($A14,Sheet2!$A$3:$H$74,F$1,)</f>
         <v>2.7334000000000001</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G14" s="6">
         <f>VLOOKUP($A14,Sheet2!$A$3:$H$74,G$1,)</f>
         <v>2.6252</v>
       </c>
-      <c r="H14" s="7">
+      <c r="H14" s="6">
         <f>VLOOKUP($A14,Sheet2!$A$3:$H$74,H$1,)</f>
         <v>2.922166666666667</v>
       </c>
-      <c r="J14" s="6" t="s">
+      <c r="J14" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="K14" s="7">
+      <c r="K14" s="6">
         <f>[1]ManSUTdet!U47*100</f>
         <v>-19.186539748694074</v>
       </c>
-      <c r="L14" s="7">
+      <c r="L14" s="6">
         <f>[1]ManSUTdet!BC47*100</f>
         <v>-0.35730794973881463</v>
       </c>
-      <c r="M14" s="7">
+      <c r="M14" s="6">
         <f>[1]ManSUTdet!BD47*100</f>
         <v>2.9199999999999995</v>
       </c>
-      <c r="N14" s="7">
+      <c r="N14" s="6">
         <f>[1]ManSUTdet!BE47*100</f>
         <v>3</v>
       </c>
-      <c r="O14" s="7">
+      <c r="O14" s="6">
         <f>[1]ManSUTdet!BF47*100</f>
         <v>3.16</v>
       </c>
-      <c r="P14" s="7">
+      <c r="P14" s="6">
         <f>[1]ManSUTdet!BG47*100</f>
         <v>3.52</v>
       </c>
-      <c r="Q14" s="7">
+      <c r="Q14" s="6">
         <f>[1]ManSUTdet!BH47*100</f>
         <v>3.7666666666666666</v>
       </c>
-      <c r="S14" s="6" t="s">
+      <c r="S14" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="T14" s="7">
+      <c r="T14" s="6">
         <f t="shared" si="8"/>
         <v>7.2725397486940739</v>
       </c>
-      <c r="U14" s="7">
+      <c r="U14" s="6">
         <f t="shared" si="2"/>
         <v>-0.3034920502611852</v>
       </c>
-      <c r="V14" s="7">
+      <c r="V14" s="6">
         <f t="shared" si="3"/>
         <v>-0.15419999999999945</v>
       </c>
-      <c r="W14" s="7">
+      <c r="W14" s="6">
         <f t="shared" si="4"/>
         <v>-0.3996000000000004</v>
       </c>
-      <c r="X14" s="7">
+      <c r="X14" s="6">
         <f t="shared" si="5"/>
         <v>-0.42660000000000009</v>
       </c>
-      <c r="Y14" s="7">
+      <c r="Y14" s="6">
         <f t="shared" si="6"/>
         <v>-0.89480000000000004</v>
       </c>
-      <c r="Z14" s="7">
+      <c r="Z14" s="6">
         <f t="shared" si="7"/>
         <v>-0.84449999999999958</v>
       </c>
     </row>
-    <row r="15" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
+    <row r="15" spans="1:39" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="6">
         <f>VLOOKUP($A15,Sheet2!$A$3:$H$74,B$1,)</f>
         <v>-10.939</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="6">
         <f>VLOOKUP($A15,Sheet2!$A$3:$H$74,C$1,)</f>
         <v>-0.16199999999999992</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="6">
         <f>VLOOKUP($A15,Sheet2!$A$3:$H$74,D$1,)</f>
         <v>2.6886000000000001</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="6">
         <f>VLOOKUP($A15,Sheet2!$A$3:$H$74,E$1,)</f>
         <v>2.6850000000000001</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="6">
         <f>VLOOKUP($A15,Sheet2!$A$3:$H$74,F$1,)</f>
         <v>2.9690000000000003</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="6">
         <f>VLOOKUP($A15,Sheet2!$A$3:$H$74,G$1,)</f>
         <v>2.9912000000000001</v>
       </c>
-      <c r="H15" s="7">
+      <c r="H15" s="6">
         <f>VLOOKUP($A15,Sheet2!$A$3:$H$74,H$1,)</f>
         <v>3.2624999999999997</v>
       </c>
-      <c r="J15" s="6" t="s">
+      <c r="J15" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="K15" s="7">
+      <c r="K15" s="6">
         <f>[1]ManSUTdet!U48*100</f>
         <v>-19.18653974869407</v>
       </c>
-      <c r="L15" s="7">
+      <c r="L15" s="6">
         <f>[1]ManSUTdet!BC48*100</f>
         <v>0.122692050261186</v>
       </c>
-      <c r="M15" s="7">
+      <c r="M15" s="6">
         <f>[1]ManSUTdet!BD48*100</f>
         <v>2.9199999999999995</v>
       </c>
-      <c r="N15" s="7">
+      <c r="N15" s="6">
         <f>[1]ManSUTdet!BE48*100</f>
         <v>3</v>
       </c>
-      <c r="O15" s="7">
+      <c r="O15" s="6">
         <f>[1]ManSUTdet!BF48*100</f>
         <v>3.16</v>
       </c>
-      <c r="P15" s="7">
+      <c r="P15" s="6">
         <f>[1]ManSUTdet!BG48*100</f>
         <v>3.52</v>
       </c>
-      <c r="Q15" s="7">
+      <c r="Q15" s="6">
         <f>[1]ManSUTdet!BH48*100</f>
         <v>3.7666666666666666</v>
       </c>
-      <c r="S15" s="6" t="s">
+      <c r="S15" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="T15" s="7">
+      <c r="T15" s="6">
         <f t="shared" si="8"/>
         <v>8.24753974869407</v>
       </c>
-      <c r="U15" s="7">
+      <c r="U15" s="6">
         <f t="shared" si="2"/>
         <v>-0.28469205026118594</v>
       </c>
-      <c r="V15" s="7">
+      <c r="V15" s="6">
         <f t="shared" si="3"/>
         <v>-0.23139999999999938</v>
       </c>
-      <c r="W15" s="7">
+      <c r="W15" s="6">
         <f t="shared" si="4"/>
         <v>-0.31499999999999995</v>
       </c>
-      <c r="X15" s="7">
+      <c r="X15" s="6">
         <f t="shared" si="5"/>
         <v>-0.19099999999999984</v>
       </c>
-      <c r="Y15" s="7">
+      <c r="Y15" s="6">
         <f t="shared" si="6"/>
         <v>-0.52879999999999994</v>
       </c>
-      <c r="Z15" s="7">
+      <c r="Z15" s="6">
         <f t="shared" si="7"/>
         <v>-0.50416666666666687</v>
       </c>
     </row>
-    <row r="16" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
+    <row r="16" spans="1:39" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="6">
         <f>VLOOKUP($A16,Sheet2!$A$3:$H$74,B$1,)</f>
         <v>-10.917999999999999</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="6">
         <f>VLOOKUP($A16,Sheet2!$A$3:$H$74,C$1,)</f>
         <v>-0.12439999999999962</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="6">
         <f>VLOOKUP($A16,Sheet2!$A$3:$H$74,D$1,)</f>
         <v>2.8073999999999999</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="6">
         <f>VLOOKUP($A16,Sheet2!$A$3:$H$74,E$1,)</f>
         <v>3.1657999999999999</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="6">
         <f>VLOOKUP($A16,Sheet2!$A$3:$H$74,F$1,)</f>
         <v>3.593</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="6">
         <f>VLOOKUP($A16,Sheet2!$A$3:$H$74,G$1,)</f>
         <v>3.7155999999999998</v>
       </c>
-      <c r="H16" s="7">
+      <c r="H16" s="6">
         <f>VLOOKUP($A16,Sheet2!$A$3:$H$74,H$1,)</f>
         <v>4.0873333333333335</v>
       </c>
-      <c r="J16" s="6" t="s">
+      <c r="J16" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="K16" s="7">
+      <c r="K16" s="6">
         <f>[1]ManSUTdet!U49*100</f>
         <v>-19.186539748694074</v>
       </c>
-      <c r="L16" s="7">
+      <c r="L16" s="6">
         <f>[1]ManSUTdet!BC49*100</f>
         <v>0.12269205026118543</v>
       </c>
-      <c r="M16" s="7">
+      <c r="M16" s="6">
         <f>[1]ManSUTdet!BD49*100</f>
         <v>2.9199999999999995</v>
       </c>
-      <c r="N16" s="7">
+      <c r="N16" s="6">
         <f>[1]ManSUTdet!BE49*100</f>
         <v>3</v>
       </c>
-      <c r="O16" s="7">
+      <c r="O16" s="6">
         <f>[1]ManSUTdet!BF49*100</f>
         <v>3.16</v>
       </c>
-      <c r="P16" s="7">
+      <c r="P16" s="6">
         <f>[1]ManSUTdet!BG49*100</f>
         <v>3.52</v>
       </c>
-      <c r="Q16" s="7">
+      <c r="Q16" s="6">
         <f>[1]ManSUTdet!BH49*100</f>
         <v>3.7666666666666666</v>
       </c>
-      <c r="S16" s="6" t="s">
+      <c r="S16" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="T16" s="7">
+      <c r="T16" s="6">
         <f t="shared" si="8"/>
         <v>8.2685397486940744</v>
       </c>
-      <c r="U16" s="7">
+      <c r="U16" s="6">
         <f t="shared" si="2"/>
         <v>-0.24709205026118505</v>
       </c>
-      <c r="V16" s="7">
+      <c r="V16" s="6">
         <f t="shared" si="3"/>
         <v>-0.11259999999999959</v>
       </c>
-      <c r="W16" s="7">
+      <c r="W16" s="6">
         <f t="shared" si="4"/>
         <v>0.16579999999999995</v>
       </c>
-      <c r="X16" s="7">
+      <c r="X16" s="6">
         <f t="shared" si="5"/>
         <v>0.43299999999999983</v>
       </c>
-      <c r="Y16" s="7">
+      <c r="Y16" s="6">
         <f t="shared" si="6"/>
         <v>0.19559999999999977</v>
       </c>
-      <c r="Z16" s="7">
+      <c r="Z16" s="6">
         <f t="shared" si="7"/>
         <v>0.32066666666666688</v>
       </c>
     </row>
-    <row r="17" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
+    <row r="17" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="6">
         <f>VLOOKUP($A17,Sheet2!$A$3:$H$74,B$1,)</f>
         <v>-10.627000000000001</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="6">
         <f>VLOOKUP($A17,Sheet2!$A$3:$H$74,C$1,)</f>
         <v>4.8799999999999691E-2</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="6">
         <f>VLOOKUP($A17,Sheet2!$A$3:$H$74,D$1,)</f>
         <v>3.2183999999999999</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="6">
         <f>VLOOKUP($A17,Sheet2!$A$3:$H$74,E$1,)</f>
         <v>2.8477999999999999</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="6">
         <f>VLOOKUP($A17,Sheet2!$A$3:$H$74,F$1,)</f>
         <v>2.8199999999999994</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="6">
         <f>VLOOKUP($A17,Sheet2!$A$3:$H$74,G$1,)</f>
         <v>2.7741999999999996</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H17" s="6">
         <f>VLOOKUP($A17,Sheet2!$A$3:$H$74,H$1,)</f>
         <v>3.0436666666666667</v>
       </c>
-      <c r="J17" s="6" t="s">
+      <c r="J17" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="K17" s="7">
+      <c r="K17" s="6">
         <f>[1]ManSUTdet!U50*100</f>
         <v>-19.186539748694077</v>
       </c>
-      <c r="L17" s="7">
+      <c r="L17" s="6">
         <f>[1]ManSUTdet!BC50*100</f>
         <v>-1.5624205590134987</v>
       </c>
-      <c r="M17" s="7">
+      <c r="M17" s="6">
         <f>[1]ManSUTdet!BD50*100</f>
         <v>1.9448868291513</v>
       </c>
-      <c r="N17" s="7">
+      <c r="N17" s="6">
         <f>[1]ManSUTdet!BE50*100</f>
         <v>2.390970093206497</v>
       </c>
-      <c r="O17" s="7">
+      <c r="O17" s="6">
         <f>[1]ManSUTdet!BF50*100</f>
         <v>2.7185270994563826</v>
       </c>
-      <c r="P17" s="7">
+      <c r="P17" s="6">
         <f>[1]ManSUTdet!BG50*100</f>
         <v>3.2367869072987077</v>
       </c>
-      <c r="Q17" s="7">
+      <c r="Q17" s="6">
         <f>[1]ManSUTdet!BH50*100</f>
         <v>3.5112670094882614</v>
       </c>
-      <c r="S17" s="6" t="s">
+      <c r="S17" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="T17" s="7">
+      <c r="T17" s="6">
         <f t="shared" si="8"/>
         <v>8.5595397486940765</v>
       </c>
-      <c r="U17" s="7">
+      <c r="U17" s="6">
         <f t="shared" si="2"/>
         <v>1.6112205590134985</v>
       </c>
-      <c r="V17" s="7">
+      <c r="V17" s="6">
         <f t="shared" si="3"/>
         <v>1.2735131708487</v>
       </c>
-      <c r="W17" s="7">
+      <c r="W17" s="6">
         <f t="shared" si="4"/>
         <v>0.45682990679350288</v>
       </c>
-      <c r="X17" s="7">
+      <c r="X17" s="6">
         <f t="shared" si="5"/>
         <v>0.1014729005436168</v>
       </c>
-      <c r="Y17" s="7">
+      <c r="Y17" s="6">
         <f t="shared" si="6"/>
         <v>-0.46258690729870811</v>
       </c>
-      <c r="Z17" s="7">
+      <c r="Z17" s="6">
         <f t="shared" si="7"/>
         <v>-0.46760034282159468</v>
       </c>

</xml_diff>